<commit_message>
remarks and questions for the Biplot and CPV plot
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/error_budget.xlsx
+++ b/_INTERPOLATION/error_budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_INTERPOLATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05E121F-09C5-43E5-B0DA-5F801055CC8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5208A86-E4B4-4BD7-B08A-CFAD00B09D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B30A4CA7-3C11-47FA-9AAE-51C8F55DE748}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
   <si>
     <t>search_radius</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Area5</t>
   </si>
   <si>
-    <t>MSPE winst</t>
-  </si>
-  <si>
     <t>area1</t>
   </si>
   <si>
@@ -87,6 +84,12 @@
   </si>
   <si>
     <t>area5</t>
+  </si>
+  <si>
+    <t>Var gain</t>
+  </si>
+  <si>
+    <t>MSPE gain</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <dimension ref="A2:AR30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +516,7 @@
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
@@ -1758,32 +1761,53 @@
       <c r="A15" s="4"/>
       <c r="J15" s="4"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>1</v>
       </c>
@@ -1802,8 +1826,26 @@
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K19" s="7">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <f>B19+1</f>
         <v>2</v>
@@ -1828,8 +1870,32 @@
         <f>(AO3-AO4)/AO4</f>
         <v>4.7611854691151555E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K20" s="7">
+        <f>K19+1</f>
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <f>(D4-D3)/D4</f>
+        <v>0.38045518591507943</v>
+      </c>
+      <c r="M20">
+        <f>(M4-M3)/M4</f>
+        <v>0.36911189693561969</v>
+      </c>
+      <c r="N20">
+        <f>(V4-V3)/V4</f>
+        <v>0.48164568193040896</v>
+      </c>
+      <c r="O20">
+        <f>(AE4-AE3)/AE4</f>
+        <v>0.28384609239213421</v>
+      </c>
+      <c r="P20">
+        <f>(AN4-AN3)/AN4</f>
+        <v>0.46133272232418193</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="7">
         <f t="shared" ref="B21:B28" si="0">B20+1</f>
         <v>3</v>
@@ -1839,11 +1905,11 @@
         <v>4.2144331508214401E-2</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:D29" si="2">(N4-N5)/N5</f>
+        <f t="shared" ref="D21:D28" si="2">(N4-N5)/N5</f>
         <v>3.2649899973051275E-2</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E27" si="3">(W4-W5)/W5</f>
+        <f t="shared" ref="E21:E26" si="3">(W4-W5)/W5</f>
         <v>3.6736520176443722E-2</v>
       </c>
       <c r="F21">
@@ -1854,8 +1920,32 @@
         <f t="shared" ref="G21:G27" si="5">(AO4-AO5)/AO5</f>
         <v>2.5213045046201057E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K21" s="7">
+        <f t="shared" ref="K21:K28" si="6">K20+1</f>
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ref="L21:L29" si="7">(D5-D4)/D5</f>
+        <v>0.23283958127561596</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ref="M21:M29" si="8">(M5-M4)/M5</f>
+        <v>0.27801070556532237</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ref="N21:N28" si="9">(V5-V4)/V5</f>
+        <v>0.2736952359242214</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ref="O21:O27" si="10">(AE5-AE4)/AE5</f>
+        <v>0.19492240494033339</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ref="P21:P27" si="11">(AN5-AN4)/AN5</f>
+        <v>0.17411054293837819</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1880,8 +1970,32 @@
         <f t="shared" si="5"/>
         <v>7.9589252993141936E-3</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K22" s="7">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" si="7"/>
+        <v>5.3881894950582779E-2</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" si="8"/>
+        <v>0.17245850129795096</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="9"/>
+        <v>0.14833490880573796</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="10"/>
+        <v>0.11044150040530185</v>
+      </c>
+      <c r="P22" s="5">
+        <f t="shared" si="11"/>
+        <v>5.1509186544809536E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1906,8 +2020,32 @@
         <f t="shared" si="5"/>
         <v>7.0587164351196847E-3</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K23" s="7">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="7"/>
+        <v>2.3361523333247512E-2</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="8"/>
+        <v>3.6988391472760548E-2</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="9"/>
+        <v>5.3076514836404728E-2</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" si="10"/>
+        <v>7.8631833762555683E-2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="11"/>
+        <v>4.1202885363976427E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1932,8 +2070,32 @@
         <f t="shared" si="5"/>
         <v>7.7087189425912323E-3</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K24" s="7">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="7"/>
+        <v>1.3243026612021392E-2</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="8"/>
+        <v>2.0389622898705675E-2</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="9"/>
+        <v>2.6092228735565427E-2</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="10"/>
+        <v>4.9809811599688635E-2</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="11"/>
+        <v>2.2188883851806486E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1958,8 +2120,32 @@
         <f t="shared" si="5"/>
         <v>3.4064334981933272E-3</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K25" s="7">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="7"/>
+        <v>3.157600238569705E-2</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="8"/>
+        <v>1.0433106573845856E-2</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="9"/>
+        <v>2.7490908581258421E-2</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="10"/>
+        <v>2.4619171460802149E-2</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="11"/>
+        <v>3.0964747730479546E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1984,8 +2170,32 @@
         <f t="shared" si="5"/>
         <v>-1.0300863623402569E-3</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K26" s="7">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="7"/>
+        <v>1.9607181039311805E-2</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="8"/>
+        <v>1.540024369903897E-2</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="9"/>
+        <v>1.7234303242695963E-2</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="10"/>
+        <v>1.5147056185333664E-2</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="11"/>
+        <v>5.3596699629129985E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2010,8 +2220,32 @@
         <f t="shared" si="5"/>
         <v>-8.4126227983984559E-4</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K27" s="7">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="7"/>
+        <v>3.0577270328409779E-2</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="8"/>
+        <v>1.5906355685431015E-2</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="9"/>
+        <v>1.953926340985198E-2</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="10"/>
+        <v>1.63781536847009E-2</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="11"/>
+        <v>2.6292417678584219E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2024,8 +2258,20 @@
         <f t="shared" si="2"/>
         <v>-2.1175184504315988E-3</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K28" s="7">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="7"/>
+        <v>3.0169196535939607E-2</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="8"/>
+        <v>1.8953615935955504E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="7">
         <f>B28+1</f>
         <v>11</v>
@@ -2038,8 +2284,20 @@
         <f>(N12-N13)/N13</f>
         <v>-5.371379238602571E-4</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K29" s="7">
+        <f>K28+1</f>
+        <v>11</v>
+      </c>
+      <c r="L29">
+        <f>(D13-D12)/D13</f>
+        <v>1.0484761734642222E-2</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="8"/>
+        <v>6.4671248235285885E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="7">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
optimizing variogram parameters area2a
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/error_budget.xlsx
+++ b/_INTERPOLATION/error_budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_INTERPOLATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B541F321-5D16-40A2-8F9C-90997414C0AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBDD042-6E1F-4AC2-A9E6-76903A15A304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B30A4CA7-3C11-47FA-9AAE-51C8F55DE748}"/>
   </bookViews>
@@ -83,13 +83,13 @@
     <t>MSPE gain</t>
   </si>
   <si>
-    <t>Area6</t>
+    <t>Area3</t>
   </si>
   <si>
-    <t>area6</t>
+    <t>Area 2a</t>
   </si>
   <si>
-    <t>Area3</t>
+    <t>area2a</t>
   </si>
 </sst>
 </file>
@@ -156,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,11 +179,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -212,6 +221,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -531,7 +546,7 @@
   <dimension ref="A2:BC30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,7 +631,7 @@
         <v>6</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="V2" s="12" t="s">
         <v>0</v>
@@ -687,28 +702,28 @@
       <c r="AT2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AV2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AV2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AW2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="AX2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AX2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BA2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BB2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BC2" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -818,26 +833,26 @@
       <c r="AT3">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV3" s="2">
+      <c r="AV3" s="14">
         <v>0</v>
       </c>
       <c r="AW3">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX3">
         <v>1</v>
       </c>
       <c r="AY3">
-        <v>0.50256551695889551</v>
+        <v>0.3135243332821549</v>
       </c>
       <c r="AZ3">
-        <v>4.3907664578498364</v>
+        <v>2.9954063794763091</v>
       </c>
       <c r="BA3">
-        <v>0.40210000000000001</v>
+        <v>0.70279999999999998</v>
       </c>
       <c r="BC3">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.3">
@@ -946,26 +961,26 @@
       <c r="AT4">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV4" s="2">
+      <c r="AV4" s="14">
         <v>1</v>
       </c>
       <c r="AW4">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX4">
         <v>2</v>
       </c>
       <c r="AY4">
-        <v>0.66280653499284425</v>
+        <v>0.38298251998665372</v>
       </c>
       <c r="AZ4">
-        <v>4.1682045684297524</v>
+        <v>2.9476851302561782</v>
       </c>
       <c r="BA4">
-        <v>1.3001</v>
+        <v>0.92720000000000002</v>
       </c>
       <c r="BC4">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.3">
@@ -1074,26 +1089,26 @@
       <c r="AT5">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV5" s="2">
+      <c r="AV5" s="14">
         <v>2</v>
       </c>
       <c r="AW5">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX5">
         <v>3</v>
       </c>
       <c r="AY5">
-        <v>0.7423871310519472</v>
+        <v>0.44056957653022139</v>
       </c>
       <c r="AZ5">
-        <v>4.1756774911279919</v>
+        <v>2.9007226778188611</v>
       </c>
       <c r="BA5">
-        <v>1.4114</v>
+        <v>1.1079399999999999</v>
       </c>
       <c r="BC5">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.3">
@@ -1202,26 +1217,26 @@
       <c r="AT6">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV6" s="2">
+      <c r="AV6" s="14">
         <v>3</v>
       </c>
       <c r="AW6">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX6">
         <v>4</v>
       </c>
       <c r="AY6">
-        <v>0.7628781440870358</v>
+        <v>0.46639236828656983</v>
       </c>
       <c r="AZ6">
-        <v>4.155595433770622</v>
+        <v>2.8925363310549952</v>
       </c>
       <c r="BA6">
-        <v>1.6114999999999999</v>
+        <v>1.30124</v>
       </c>
       <c r="BC6">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="7" spans="1:55" x14ac:dyDescent="0.3">
@@ -1330,26 +1345,26 @@
       <c r="AT7">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV7" s="2">
+      <c r="AV7" s="14">
         <v>4</v>
       </c>
       <c r="AW7">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX7">
         <v>5</v>
       </c>
       <c r="AY7">
-        <v>0.78330413927710496</v>
+        <v>0.48175799781117462</v>
       </c>
       <c r="AZ7">
-        <v>4.1342699472783684</v>
+        <v>2.888593606065291</v>
       </c>
       <c r="BA7">
-        <v>1.8039000000000001</v>
+        <v>1.4191400000000001</v>
       </c>
       <c r="BC7">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.3">
@@ -1458,26 +1473,26 @@
       <c r="AT8">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV8" s="2">
+      <c r="AV8" s="14">
         <v>5</v>
       </c>
       <c r="AW8">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX8">
         <v>6</v>
       </c>
       <c r="AY8">
-        <v>0.78911886350317517</v>
+        <v>0.49471381023515693</v>
       </c>
       <c r="AZ8">
-        <v>4.1311647529014728</v>
+        <v>2.8804926344385868</v>
       </c>
       <c r="BA8">
-        <v>1.9571000000000001</v>
+        <v>1.54254</v>
       </c>
       <c r="BC8">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="9" spans="1:55" x14ac:dyDescent="0.3">
@@ -1586,26 +1601,26 @@
       <c r="AT9">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV9" s="2">
+      <c r="AV9" s="14">
         <v>6</v>
       </c>
       <c r="AW9">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX9">
         <v>7</v>
       </c>
       <c r="AY9">
-        <v>0.80458143034257912</v>
+        <v>0.51339599194252106</v>
       </c>
       <c r="AZ9">
-        <v>4.1216865389879196</v>
+        <v>2.8635889594376751</v>
       </c>
       <c r="BA9">
-        <v>2.0281799999999999</v>
+        <v>1.5974999999999999</v>
       </c>
       <c r="BC9">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.3">
@@ -1714,26 +1729,26 @@
       <c r="AT10">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV10" s="2">
+      <c r="AV10" s="14">
         <v>7</v>
       </c>
       <c r="AW10">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX10">
         <v>8</v>
       </c>
       <c r="AY10">
-        <v>0.80717531674573884</v>
+        <v>0.51969332790896883</v>
       </c>
       <c r="AZ10">
-        <v>4.1208121840796119</v>
+        <v>2.8618594153307289</v>
       </c>
       <c r="BA10">
-        <v>2.1436799999999998</v>
+        <v>1.6208450000000001</v>
       </c>
       <c r="BC10">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.3">
@@ -1842,26 +1857,26 @@
       <c r="AT11">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV11" s="2">
+      <c r="AV11" s="14">
         <v>8</v>
       </c>
       <c r="AW11">
-        <v>100000</v>
+        <v>25000</v>
       </c>
       <c r="AX11">
         <v>9</v>
       </c>
       <c r="AY11">
-        <v>0.81501240390430063</v>
+        <v>0.52078218128686538</v>
       </c>
       <c r="AZ11">
-        <v>4.112520540372838</v>
+        <v>2.8626624943766159</v>
       </c>
       <c r="BA11">
-        <v>2.19781</v>
+        <v>1.629678</v>
       </c>
       <c r="BC11">
-        <v>4.7976927628955961</v>
+        <v>3.226396680182666</v>
       </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.3">
@@ -1908,7 +1923,7 @@
         <v>13</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M18" s="5" t="s">
         <v>1</v>
@@ -1995,9 +2010,9 @@
         <f>(AQ3-AQ4)/AQ4</f>
         <v>1.1042853717827929E-2</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="7">
         <f>(AZ3-AZ4)/AZ4</f>
-        <v>5.3395145503601721E-2</v>
+        <v>1.6189398497926916E-2</v>
       </c>
       <c r="M20" s="6">
         <f>M19+1</f>
@@ -2049,32 +2064,32 @@
         <f t="shared" ref="G21:G27" si="2">(AQ4-AQ5)/AQ5</f>
         <v>2.0090557373475284E-2</v>
       </c>
-      <c r="H21">
-        <f t="shared" ref="H21:H27" si="3">(AZ4-AZ5)/AZ5</f>
-        <v>-1.7896311949658797E-3</v>
+      <c r="H21" s="4">
+        <f>(AZ4-AZ5)/AZ5</f>
+        <v>1.6189914601774193E-2</v>
       </c>
       <c r="M21" s="6">
-        <f t="shared" ref="M21:M28" si="4">M20+1</f>
+        <f t="shared" ref="M21:M28" si="3">M20+1</f>
         <v>3</v>
       </c>
       <c r="N21">
-        <f t="shared" ref="N21:N27" si="5">(D5-D4)/D5</f>
+        <f t="shared" ref="N21:N27" si="4">(D5-D4)/D5</f>
         <v>0.10176566872127661</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="O21:O29" si="6">(O5-O4)/O5</f>
+        <f t="shared" ref="O21:O29" si="5">(O5-O4)/O5</f>
         <v>8.5557354256765014E-2</v>
       </c>
       <c r="P21">
-        <f t="shared" ref="P21:P27" si="7">(X5-X4)/X5</f>
+        <f t="shared" ref="P21:P27" si="6">(X5-X4)/X5</f>
         <v>7.1481595096278494E-2</v>
       </c>
       <c r="Q21">
-        <f t="shared" ref="Q21:Q27" si="8">(AG5-AG4)/AG5</f>
+        <f t="shared" ref="Q21:Q27" si="7">(AG5-AG4)/AG5</f>
         <v>9.773195075543345E-2</v>
       </c>
       <c r="R21">
-        <f t="shared" ref="R21:R27" si="9">(AP5-AP4)/AP5</f>
+        <f t="shared" ref="R21:R27" si="8">(AP5-AP4)/AP5</f>
         <v>0.21229867917953107</v>
       </c>
     </row>
@@ -2088,11 +2103,11 @@
         <v>6.0519930267361223E-3</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" ref="D22:D27" si="10">(P5-P6)/P6</f>
+        <f t="shared" ref="D22:D27" si="9">(P5-P6)/P6</f>
         <v>9.1718676206817111E-4</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" ref="E22:E26" si="11">(Y5-Y6)/Y6</f>
+        <f t="shared" ref="E22:E26" si="10">(Y5-Y6)/Y6</f>
         <v>8.3788475357532057E-3</v>
       </c>
       <c r="F22" s="4">
@@ -2104,31 +2119,31 @@
         <v>-2.7003661730892947E-3</v>
       </c>
       <c r="H22">
+        <f t="shared" ref="H21:H27" si="11">(AZ5-AZ6)/AZ6</f>
+        <v>2.830162123108083E-3</v>
+      </c>
+      <c r="M22" s="6">
         <f t="shared" si="3"/>
-        <v>4.8325342727475852E-3</v>
-      </c>
-      <c r="M22" s="6">
+        <v>4</v>
+      </c>
+      <c r="N22" s="4">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="N22" s="4">
+        <v>7.6646158209822388E-2</v>
+      </c>
+      <c r="O22" s="4">
         <f t="shared" si="5"/>
-        <v>7.6646158209822388E-2</v>
-      </c>
-      <c r="O22" s="4">
+        <v>5.8682521593663856E-2</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="6"/>
-        <v>5.8682521593663856E-2</v>
-      </c>
-      <c r="P22">
+        <v>7.2696141264064873E-2</v>
+      </c>
+      <c r="Q22">
         <f t="shared" si="7"/>
-        <v>7.2696141264064873E-2</v>
-      </c>
-      <c r="Q22">
+        <v>0.16708960155030728</v>
+      </c>
+      <c r="R22" s="4">
         <f t="shared" si="8"/>
-        <v>0.16708960155030728</v>
-      </c>
-      <c r="R22" s="4">
-        <f t="shared" si="9"/>
         <v>5.9839952835964098E-2</v>
       </c>
     </row>
@@ -2142,11 +2157,11 @@
         <v>1.2553697719539917E-3</v>
       </c>
       <c r="D23">
+        <f t="shared" si="9"/>
+        <v>-2.8219906800217784E-3</v>
+      </c>
+      <c r="E23">
         <f t="shared" si="10"/>
-        <v>-2.8219906800217784E-3</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="11"/>
         <v>3.2751722261865736E-3</v>
       </c>
       <c r="F23" s="7">
@@ -2158,31 +2173,31 @@
         <v>9.7996902403431237E-3</v>
       </c>
       <c r="H23">
+        <f t="shared" si="11"/>
+        <v>1.3649289333831764E-3</v>
+      </c>
+      <c r="M23" s="6">
         <f t="shared" si="3"/>
-        <v>5.1582230391831125E-3</v>
-      </c>
-      <c r="M23" s="6">
+        <v>5</v>
+      </c>
+      <c r="N23">
         <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="N23">
+        <v>4.9151504423963835E-2</v>
+      </c>
+      <c r="O23">
         <f t="shared" si="5"/>
-        <v>4.9151504423963835E-2</v>
-      </c>
-      <c r="O23">
+        <v>3.0016184734596496E-2</v>
+      </c>
+      <c r="P23" s="4">
         <f t="shared" si="6"/>
-        <v>3.0016184734596496E-2</v>
-      </c>
-      <c r="P23" s="4">
+        <v>5.3218237177546097E-2</v>
+      </c>
+      <c r="Q23" s="4">
         <f t="shared" si="7"/>
-        <v>5.3218237177546097E-2</v>
-      </c>
-      <c r="Q23" s="4">
+        <v>3.899768779105587E-2</v>
+      </c>
+      <c r="R23">
         <f t="shared" si="8"/>
-        <v>3.899768779105587E-2</v>
-      </c>
-      <c r="R23">
-        <f t="shared" si="9"/>
         <v>7.4313676922907565E-2</v>
       </c>
     </row>
@@ -2196,7 +2211,7 @@
         <v>5.5331216924087842E-3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-6.4551222529511492E-4</v>
       </c>
       <c r="E24">
@@ -2212,31 +2227,31 @@
         <v>-3.2183711518570545E-3</v>
       </c>
       <c r="H24">
+        <f t="shared" si="11"/>
+        <v>2.8123563066437401E-3</v>
+      </c>
+      <c r="M24" s="6">
         <f t="shared" si="3"/>
-        <v>7.5165106274561154E-4</v>
-      </c>
-      <c r="M24" s="6">
+        <v>6</v>
+      </c>
+      <c r="N24">
         <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="N24">
+        <v>4.2686815096649983E-2</v>
+      </c>
+      <c r="O24">
         <f t="shared" si="5"/>
-        <v>4.2686815096649983E-2</v>
-      </c>
-      <c r="O24">
+        <v>4.4278249967540102E-2</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="6"/>
-        <v>4.4278249967540102E-2</v>
-      </c>
-      <c r="P24">
+        <v>3.9822575755710674E-2</v>
+      </c>
+      <c r="Q24">
         <f t="shared" si="7"/>
-        <v>3.9822575755710674E-2</v>
-      </c>
-      <c r="Q24">
+        <v>1.8254949408081911E-2</v>
+      </c>
+      <c r="R24">
         <f t="shared" si="8"/>
-        <v>1.8254949408081911E-2</v>
-      </c>
-      <c r="R24">
-        <f t="shared" si="9"/>
         <v>2.620127547567833E-2</v>
       </c>
     </row>
@@ -2250,11 +2265,11 @@
         <v>1.0474507201882914E-2</v>
       </c>
       <c r="D25">
+        <f t="shared" si="9"/>
+        <v>1.8539505663454855E-3</v>
+      </c>
+      <c r="E25">
         <f t="shared" si="10"/>
-        <v>1.8539505663454855E-3</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="11"/>
         <v>7.6313763388460958E-3</v>
       </c>
       <c r="F25">
@@ -2266,31 +2281,31 @@
         <v>-2.941055980213555E-3</v>
       </c>
       <c r="H25">
+        <f t="shared" si="11"/>
+        <v>5.9029683520749106E-3</v>
+      </c>
+      <c r="M25" s="6">
         <f t="shared" si="3"/>
-        <v>2.2995960085505597E-3</v>
-      </c>
-      <c r="M25" s="6">
+        <v>7</v>
+      </c>
+      <c r="N25">
         <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="N25">
+        <v>4.4785647777125841E-2</v>
+      </c>
+      <c r="O25">
         <f t="shared" si="5"/>
-        <v>4.4785647777125841E-2</v>
-      </c>
-      <c r="O25">
+        <v>3.4152860871484746E-2</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="6"/>
-        <v>3.4152860871484746E-2</v>
-      </c>
-      <c r="P25">
+        <v>3.8026372244194445E-2</v>
+      </c>
+      <c r="Q25">
         <f t="shared" si="7"/>
-        <v>3.8026372244194445E-2</v>
-      </c>
-      <c r="Q25">
+        <v>2.5035106576661761E-2</v>
+      </c>
+      <c r="R25">
         <f t="shared" si="8"/>
-        <v>2.5035106576661761E-2</v>
-      </c>
-      <c r="R25">
-        <f t="shared" si="9"/>
         <v>1.0543091480369964E-2</v>
       </c>
     </row>
@@ -2308,7 +2323,7 @@
         <v>7.8479949475812312E-4</v>
       </c>
       <c r="E26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>2.32010104704502E-3</v>
       </c>
       <c r="F26">
@@ -2320,31 +2335,31 @@
         <v>1.4184803600365327E-3</v>
       </c>
       <c r="H26">
+        <f t="shared" si="11"/>
+        <v>6.0434279115222837E-4</v>
+      </c>
+      <c r="M26" s="6">
         <f t="shared" si="3"/>
-        <v>2.1218023759628373E-4</v>
-      </c>
-      <c r="M26" s="6">
+        <v>8</v>
+      </c>
+      <c r="N26">
         <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="N26">
+        <v>9.7504489348369978E-3</v>
+      </c>
+      <c r="O26">
         <f t="shared" si="5"/>
-        <v>9.7504489348369978E-3</v>
-      </c>
-      <c r="O26">
+        <v>1.2852928851536664E-2</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="6"/>
-        <v>1.2852928851536664E-2</v>
-      </c>
-      <c r="P26">
+        <v>1.4997704246726501E-2</v>
+      </c>
+      <c r="Q26">
         <f t="shared" si="7"/>
-        <v>1.4997704246726501E-2</v>
-      </c>
-      <c r="Q26">
+        <v>2.3023925946269997E-2</v>
+      </c>
+      <c r="R26">
         <f t="shared" si="8"/>
-        <v>2.3023925946269997E-2</v>
-      </c>
-      <c r="R26">
-        <f t="shared" si="9"/>
         <v>2.3277044875244048E-2</v>
       </c>
     </row>
@@ -2358,7 +2373,7 @@
         <v>1.0028820484149271E-3</v>
       </c>
       <c r="D27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>3.1752462770683504E-4</v>
       </c>
       <c r="E27">
@@ -2374,31 +2389,31 @@
         <v>-5.9897149380518581E-5</v>
       </c>
       <c r="H27">
+        <f t="shared" si="11"/>
+        <v>-2.8053570669424576E-4</v>
+      </c>
+      <c r="M27" s="6">
         <f t="shared" si="3"/>
-        <v>2.0161950865349885E-3</v>
-      </c>
-      <c r="M27" s="6">
+        <v>9</v>
+      </c>
+      <c r="N27">
         <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="N27">
+        <v>4.4282359502808418E-3</v>
+      </c>
+      <c r="O27">
         <f t="shared" si="5"/>
-        <v>4.4282359502808418E-3</v>
-      </c>
-      <c r="O27">
+        <v>5.0659100638200602E-3</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="6"/>
-        <v>5.0659100638200602E-3</v>
-      </c>
-      <c r="P27">
+        <v>7.6460337820037638E-3</v>
+      </c>
+      <c r="Q27">
         <f t="shared" si="7"/>
-        <v>7.6460337820037638E-3</v>
-      </c>
-      <c r="Q27">
+        <v>5.7068466060010122E-3</v>
+      </c>
+      <c r="R27">
         <f t="shared" si="8"/>
-        <v>5.7068466060010122E-3</v>
-      </c>
-      <c r="R27">
-        <f t="shared" si="9"/>
         <v>1.6803715234263625E-3</v>
       </c>
     </row>
@@ -2408,11 +2423,11 @@
         <v>10</v>
       </c>
       <c r="M28" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="O28" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2426,7 +2441,7 @@
         <v>11</v>
       </c>
       <c r="O29" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optimizing variogram parameters area2b
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/error_budget.xlsx
+++ b/_INTERPOLATION/error_budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_INTERPOLATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBDD042-6E1F-4AC2-A9E6-76903A15A304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9009CC9A-6CEB-461A-B165-1DD515808FA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B30A4CA7-3C11-47FA-9AAE-51C8F55DE748}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
   <si>
     <t>search_radius</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>area2a</t>
+  </si>
+  <si>
+    <t>area2b</t>
+  </si>
+  <si>
+    <t>Area 2b</t>
   </si>
 </sst>
 </file>
@@ -192,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -221,9 +227,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671D0FF-6F7B-4180-8916-6B2747DEAF8E}">
-  <dimension ref="A2:BC30"/>
+  <dimension ref="A2:BN30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,34 +560,34 @@
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="12" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="12" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="12" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="12" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -609,125 +612,151 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="M2" s="1" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="O2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="X2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="12" t="s">
+      <c r="Y2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="12" t="s">
+      <c r="AA2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="AB2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AC2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AD2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AF2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="12" t="s">
+      <c r="AG2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AF2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="12" t="s">
+      <c r="AH2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AJ2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AK2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="12" t="s">
+      <c r="AL2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AK2" s="12" t="s">
+      <c r="AM2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AO2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AN2" s="12" t="s">
+      <c r="AP2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AO2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP2" s="12" t="s">
+      <c r="AQ2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AQ2" s="12" t="s">
+      <c r="AS2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AR2" s="12" t="s">
+      <c r="AT2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AS2" s="12" t="s">
+      <c r="AU2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AT2" s="12" t="s">
+      <c r="AV2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AV2" s="15" t="s">
+      <c r="AX2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AW2" s="14" t="s">
+      <c r="AY2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AX2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="AY2" s="14" t="s">
+      <c r="AZ2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AZ2" s="14" t="s">
+      <c r="BB2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="BA2" s="14" t="s">
+      <c r="BC2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="BB2" s="14" t="s">
+      <c r="BD2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="BC2" s="14" t="s">
+      <c r="BE2" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="BG2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="BH2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="BL2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="BN2" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>0</v>
       </c>
@@ -749,113 +778,134 @@
       <c r="H3">
         <v>2.995599830918374</v>
       </c>
-      <c r="L3" s="2">
+      <c r="N3" s="2">
         <v>0</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>50000</v>
       </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>0.48067336594687038</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>3.7283063930572342</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>0.95240000000000002</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U3" s="13">
+      <c r="W3" s="13">
         <v>0</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>75000</v>
       </c>
-      <c r="W3">
-        <v>1</v>
-      </c>
-      <c r="X3">
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
         <v>0.38033031902469272</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>3.6025795623284291</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>0.75180000000000002</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD3" s="13">
+      <c r="AF3" s="13">
         <v>0</v>
       </c>
-      <c r="AE3">
+      <c r="AG3">
         <v>90000</v>
       </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
-      <c r="AG3">
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
         <v>0.53794659513894327</v>
       </c>
-      <c r="AH3">
+      <c r="AJ3">
         <v>3.296988220851615</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>1.006</v>
       </c>
-      <c r="AK3">
+      <c r="AM3">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM3" s="13">
+      <c r="AO3" s="13">
         <v>0</v>
       </c>
-      <c r="AN3">
+      <c r="AP3">
         <v>70000</v>
       </c>
-      <c r="AO3">
-        <v>1</v>
-      </c>
-      <c r="AP3">
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
         <v>0.44461726443180999</v>
       </c>
-      <c r="AQ3">
+      <c r="AS3">
         <v>4.0161955823321929</v>
       </c>
-      <c r="AR3">
+      <c r="AT3">
         <v>0.68979999999999997</v>
       </c>
-      <c r="AT3">
+      <c r="AV3">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV3" s="14">
+      <c r="AX3" s="13">
         <v>0</v>
       </c>
-      <c r="AW3">
+      <c r="AY3">
         <v>25000</v>
       </c>
-      <c r="AX3">
-        <v>1</v>
-      </c>
-      <c r="AY3">
+      <c r="AZ3">
+        <v>1</v>
+      </c>
+      <c r="BA3">
         <v>0.3135243332821549</v>
       </c>
-      <c r="AZ3">
+      <c r="BB3">
         <v>2.9954063794763091</v>
       </c>
-      <c r="BA3">
+      <c r="BC3">
         <v>0.70279999999999998</v>
       </c>
-      <c r="BC3">
+      <c r="BE3">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG3" s="13">
+        <v>0</v>
+      </c>
+      <c r="BH3">
+        <v>22500</v>
+      </c>
+      <c r="BI3">
+        <v>1</v>
+      </c>
+      <c r="BJ3">
+        <v>0.22445657144535569</v>
+      </c>
+      <c r="BK3">
+        <v>4.2051235592021188</v>
+      </c>
+      <c r="BL3">
+        <v>1.3351999999999999</v>
+      </c>
+      <c r="BN3">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -877,113 +927,134 @@
       <c r="H4">
         <v>2.995599830918374</v>
       </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4">
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>50000</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>2</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>0.76520614282182042</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>3.6058896144473729</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>1.4483999999999999</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U4" s="13">
-        <v>1</v>
-      </c>
-      <c r="V4">
+      <c r="W4" s="13">
+        <v>1</v>
+      </c>
+      <c r="X4">
         <v>75000</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>2</v>
       </c>
-      <c r="X4">
+      <c r="Z4">
         <v>0.69008680305220649</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>3.3636685309936909</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>1.3849</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD4" s="13">
-        <v>1</v>
-      </c>
-      <c r="AE4">
+      <c r="AF4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AG4">
         <v>90000</v>
       </c>
-      <c r="AF4">
+      <c r="AH4">
         <v>2</v>
       </c>
-      <c r="AG4">
+      <c r="AI4">
         <v>0.72813774884466864</v>
       </c>
-      <c r="AH4">
+      <c r="AJ4">
         <v>3.1505799926727289</v>
       </c>
-      <c r="AI4">
+      <c r="AK4">
         <v>1.4530000000000001</v>
       </c>
-      <c r="AK4">
+      <c r="AM4">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM4" s="13">
-        <v>1</v>
-      </c>
-      <c r="AN4">
+      <c r="AO4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AP4">
         <v>70000</v>
       </c>
-      <c r="AO4">
+      <c r="AQ4">
         <v>2</v>
       </c>
-      <c r="AP4">
+      <c r="AR4">
         <v>0.60043816217184121</v>
       </c>
-      <c r="AQ4">
+      <c r="AS4">
         <v>3.9723297262462758</v>
       </c>
-      <c r="AR4">
+      <c r="AT4">
         <v>1.1192</v>
       </c>
-      <c r="AT4">
+      <c r="AV4">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV4" s="14">
-        <v>1</v>
-      </c>
-      <c r="AW4">
+      <c r="AX4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AY4">
         <v>25000</v>
       </c>
-      <c r="AX4">
+      <c r="AZ4">
         <v>2</v>
       </c>
-      <c r="AY4">
+      <c r="BA4">
         <v>0.38298251998665372</v>
       </c>
-      <c r="AZ4">
+      <c r="BB4">
         <v>2.9476851302561782</v>
       </c>
-      <c r="BA4">
+      <c r="BC4">
         <v>0.92720000000000002</v>
       </c>
-      <c r="BC4">
+      <c r="BE4">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG4" s="13">
+        <v>1</v>
+      </c>
+      <c r="BH4">
+        <v>22500</v>
+      </c>
+      <c r="BI4">
+        <v>2</v>
+      </c>
+      <c r="BJ4">
+        <v>0.36957190579716998</v>
+      </c>
+      <c r="BK4">
+        <v>4.1280536110648516</v>
+      </c>
+      <c r="BL4">
+        <v>1.8603000000000001</v>
+      </c>
+      <c r="BN4">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>2</v>
       </c>
@@ -1005,113 +1076,134 @@
       <c r="H5">
         <v>2.995599830918374</v>
       </c>
-      <c r="L5" s="2">
+      <c r="N5" s="2">
         <v>2</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>50000</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>3</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>0.83680058709409921</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>3.600120342288808</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>1.7071000000000001</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U5" s="13">
+      <c r="W5" s="13">
         <v>2</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>75000</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>3</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>0.74321284253246644</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>3.3523063974154081</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>1.7165999999999999</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD5" s="13">
+      <c r="AF5" s="13">
         <v>2</v>
       </c>
-      <c r="AE5">
+      <c r="AG5">
         <v>90000</v>
       </c>
-      <c r="AF5">
+      <c r="AH5">
         <v>3</v>
       </c>
-      <c r="AG5">
+      <c r="AI5">
         <v>0.80700823824395607</v>
       </c>
-      <c r="AH5">
+      <c r="AJ5">
         <v>3.14240151487407</v>
       </c>
-      <c r="AI5">
+      <c r="AK5">
         <v>1.7876000000000001</v>
       </c>
-      <c r="AK5">
+      <c r="AM5">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM5" s="13">
+      <c r="AO5" s="13">
         <v>2</v>
       </c>
-      <c r="AN5">
+      <c r="AP5">
         <v>70000</v>
       </c>
-      <c r="AO5">
+      <c r="AQ5">
         <v>3</v>
       </c>
-      <c r="AP5">
+      <c r="AR5">
         <v>0.76226628837745936</v>
       </c>
-      <c r="AQ5">
+      <c r="AS5">
         <v>3.8940951835435209</v>
       </c>
-      <c r="AR5">
+      <c r="AT5">
         <v>1.6471</v>
       </c>
-      <c r="AT5">
+      <c r="AV5">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV5" s="14">
+      <c r="AX5" s="13">
         <v>2</v>
       </c>
-      <c r="AW5">
+      <c r="AY5">
         <v>25000</v>
       </c>
-      <c r="AX5">
+      <c r="AZ5">
         <v>3</v>
       </c>
-      <c r="AY5">
+      <c r="BA5">
         <v>0.44056957653022139</v>
       </c>
-      <c r="AZ5">
+      <c r="BB5">
         <v>2.9007226778188611</v>
       </c>
-      <c r="BA5">
+      <c r="BC5">
         <v>1.1079399999999999</v>
       </c>
-      <c r="BC5">
+      <c r="BE5">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG5" s="13">
+        <v>2</v>
+      </c>
+      <c r="BH5">
+        <v>22500</v>
+      </c>
+      <c r="BI5">
+        <v>3</v>
+      </c>
+      <c r="BJ5">
+        <v>0.42531097324201539</v>
+      </c>
+      <c r="BK5">
+        <v>4.1857187989251718</v>
+      </c>
+      <c r="BL5">
+        <v>2.3582999999999998</v>
+      </c>
+      <c r="BN5">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -1133,113 +1225,134 @@
       <c r="H6">
         <v>2.995599830918374</v>
       </c>
-      <c r="L6" s="2">
+      <c r="N6" s="2">
         <v>3</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>50000</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>4</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>0.88896743796876532</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>3.5968213853286608</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>1.9228000000000001</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U6" s="13">
+      <c r="W6" s="13">
         <v>3</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>75000</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>4</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>0.80147713775890628</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>3.3244513266097129</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <v>1.95</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD6" s="13">
+      <c r="AF6" s="13">
         <v>3</v>
       </c>
-      <c r="AE6">
+      <c r="AG6">
         <v>90000</v>
       </c>
-      <c r="AF6">
+      <c r="AH6">
         <v>4</v>
       </c>
-      <c r="AG6">
+      <c r="AI6">
         <v>0.96890162464780283</v>
       </c>
-      <c r="AH6">
+      <c r="AJ6">
         <v>3.0602980466926861</v>
       </c>
-      <c r="AI6">
+      <c r="AK6">
         <v>1.9857</v>
       </c>
-      <c r="AK6">
+      <c r="AM6">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM6" s="13">
+      <c r="AO6" s="13">
         <v>3</v>
       </c>
-      <c r="AN6">
+      <c r="AP6">
         <v>70000</v>
       </c>
-      <c r="AO6">
+      <c r="AQ6">
         <v>4</v>
       </c>
-      <c r="AP6">
+      <c r="AR6">
         <v>0.81078353699118821</v>
       </c>
-      <c r="AQ6">
+      <c r="AS6">
         <v>3.904639138992577</v>
       </c>
-      <c r="AR6">
+      <c r="AT6">
         <v>1.9302999999999999</v>
       </c>
-      <c r="AT6">
+      <c r="AV6">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV6" s="14">
+      <c r="AX6" s="13">
         <v>3</v>
       </c>
-      <c r="AW6">
+      <c r="AY6">
         <v>25000</v>
       </c>
-      <c r="AX6">
+      <c r="AZ6">
         <v>4</v>
       </c>
-      <c r="AY6">
+      <c r="BA6">
         <v>0.46639236828656983</v>
       </c>
-      <c r="AZ6">
+      <c r="BB6">
         <v>2.8925363310549952</v>
       </c>
-      <c r="BA6">
+      <c r="BC6">
         <v>1.30124</v>
       </c>
-      <c r="BC6">
+      <c r="BE6">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG6" s="13">
+        <v>3</v>
+      </c>
+      <c r="BH6">
+        <v>22500</v>
+      </c>
+      <c r="BI6">
+        <v>4</v>
+      </c>
+      <c r="BJ6">
+        <v>0.52555379164144767</v>
+      </c>
+      <c r="BK6">
+        <v>4.1527969844867956</v>
+      </c>
+      <c r="BL6">
+        <v>2.5823999999999998</v>
+      </c>
+      <c r="BN6">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>4</v>
       </c>
@@ -1261,113 +1374,134 @@
       <c r="H7">
         <v>2.995599830918374</v>
       </c>
-      <c r="L7" s="2">
+      <c r="N7" s="2">
         <v>4</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>50000</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>5</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>0.91647656793688792</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>3.6070003065766558</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>2.1351</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U7" s="13">
+      <c r="W7" s="13">
         <v>4</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>75000</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <v>5</v>
       </c>
-      <c r="X7">
+      <c r="Z7">
         <v>0.84652785808803543</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>3.3135987201128718</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <v>2.0798000000000001</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD7" s="13">
+      <c r="AF7" s="13">
         <v>4</v>
       </c>
-      <c r="AE7">
+      <c r="AG7">
         <v>90000</v>
       </c>
-      <c r="AF7">
+      <c r="AH7">
         <v>5</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>1.0082198682963639</v>
       </c>
-      <c r="AH7">
+      <c r="AJ7">
         <v>3.0512501356848012</v>
       </c>
-      <c r="AI7">
+      <c r="AK7">
         <v>2.1518999999999999</v>
       </c>
-      <c r="AK7">
+      <c r="AM7">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM7" s="13">
+      <c r="AO7" s="13">
         <v>4</v>
       </c>
-      <c r="AN7">
+      <c r="AP7">
         <v>70000</v>
       </c>
-      <c r="AO7">
+      <c r="AQ7">
         <v>5</v>
       </c>
-      <c r="AP7">
+      <c r="AR7">
         <v>0.87587287051627427</v>
       </c>
-      <c r="AQ7">
+      <c r="AS7">
         <v>3.8667462237616959</v>
       </c>
-      <c r="AR7">
+      <c r="AT7">
         <v>2.01986</v>
       </c>
-      <c r="AT7">
+      <c r="AV7">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV7" s="14">
+      <c r="AX7" s="13">
         <v>4</v>
       </c>
-      <c r="AW7">
+      <c r="AY7">
         <v>25000</v>
       </c>
-      <c r="AX7">
+      <c r="AZ7">
         <v>5</v>
       </c>
-      <c r="AY7">
+      <c r="BA7">
         <v>0.48175799781117462</v>
       </c>
-      <c r="AZ7">
+      <c r="BB7">
         <v>2.888593606065291</v>
       </c>
-      <c r="BA7">
+      <c r="BC7">
         <v>1.4191400000000001</v>
       </c>
-      <c r="BC7">
+      <c r="BE7">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG7" s="13">
+        <v>4</v>
+      </c>
+      <c r="BH7">
+        <v>22500</v>
+      </c>
+      <c r="BI7">
+        <v>5</v>
+      </c>
+      <c r="BJ7">
+        <v>0.56381355508322006</v>
+      </c>
+      <c r="BK7">
+        <v>4.1740647229724948</v>
+      </c>
+      <c r="BL7">
+        <v>2.8435000000000001</v>
+      </c>
+      <c r="BN7">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -1389,113 +1523,134 @@
       <c r="H8">
         <v>2.995599830918374</v>
       </c>
-      <c r="L8" s="2">
+      <c r="N8" s="2">
         <v>5</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>50000</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>6</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>0.95893660252658364</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>3.609330173328666</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>2.3302999999999998</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U8" s="13">
+      <c r="W8" s="13">
         <v>5</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>75000</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <v>6</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <v>0.88163691075563233</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <v>3.3051287071358479</v>
       </c>
-      <c r="Z8">
+      <c r="AB8">
         <v>2.2050000000000001</v>
       </c>
-      <c r="AB8">
+      <c r="AD8">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD8" s="13">
+      <c r="AF8" s="13">
         <v>5</v>
       </c>
-      <c r="AE8">
+      <c r="AG8">
         <v>90000</v>
       </c>
-      <c r="AF8">
+      <c r="AH8">
         <v>6</v>
       </c>
-      <c r="AG8">
+      <c r="AI8">
         <v>1.026967100764586</v>
       </c>
-      <c r="AH8">
+      <c r="AJ8">
         <v>3.0533007950275342</v>
       </c>
-      <c r="AI8">
+      <c r="AK8">
         <v>2.2700999999999998</v>
       </c>
-      <c r="AK8">
+      <c r="AM8">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM8" s="13">
+      <c r="AO8" s="13">
         <v>5</v>
       </c>
-      <c r="AN8">
+      <c r="AP8">
         <v>70000</v>
       </c>
-      <c r="AO8">
+      <c r="AQ8">
         <v>6</v>
       </c>
-      <c r="AP8">
+      <c r="AR8">
         <v>0.899439328126167</v>
       </c>
-      <c r="AQ8">
+      <c r="AS8">
         <v>3.8792310289968079</v>
       </c>
-      <c r="AR8">
+      <c r="AT8">
         <v>2.1240600000000001</v>
       </c>
-      <c r="AT8">
+      <c r="AV8">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV8" s="14">
+      <c r="AX8" s="13">
         <v>5</v>
       </c>
-      <c r="AW8">
+      <c r="AY8">
         <v>25000</v>
       </c>
-      <c r="AX8">
+      <c r="AZ8">
         <v>6</v>
       </c>
-      <c r="AY8">
+      <c r="BA8">
         <v>0.49471381023515693</v>
       </c>
-      <c r="AZ8">
+      <c r="BB8">
         <v>2.8804926344385868</v>
       </c>
-      <c r="BA8">
+      <c r="BC8">
         <v>1.54254</v>
       </c>
-      <c r="BC8">
+      <c r="BE8">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG8" s="13">
+        <v>5</v>
+      </c>
+      <c r="BH8">
+        <v>22500</v>
+      </c>
+      <c r="BI8">
+        <v>6</v>
+      </c>
+      <c r="BJ8">
+        <v>0.59448430017612008</v>
+      </c>
+      <c r="BK8">
+        <v>4.2014789529715211</v>
+      </c>
+      <c r="BL8">
+        <v>3.0501</v>
+      </c>
+      <c r="BN8">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>6</v>
       </c>
@@ -1517,113 +1672,134 @@
       <c r="H9">
         <v>2.995599830918374</v>
       </c>
-      <c r="L9" s="2">
+      <c r="N9" s="2">
         <v>6</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>50000</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>7</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>0.99284510320321806</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>3.6026510363993882</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>2.4392999999999998</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U9" s="13">
+      <c r="W9" s="13">
         <v>6</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>75000</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <v>7</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>0.91648760976161969</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>3.2800970521033079</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>2.3134000000000001</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD9" s="13">
+      <c r="AF9" s="13">
         <v>6</v>
       </c>
-      <c r="AE9">
+      <c r="AG9">
         <v>90000</v>
       </c>
-      <c r="AF9">
+      <c r="AH9">
         <v>7</v>
       </c>
-      <c r="AG9">
+      <c r="AI9">
         <v>1.053337517783492</v>
       </c>
-      <c r="AH9">
+      <c r="AJ9">
         <v>3.050403551110147</v>
       </c>
-      <c r="AI9">
+      <c r="AK9">
         <v>2.3786</v>
       </c>
-      <c r="AK9">
+      <c r="AM9">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM9" s="13">
+      <c r="AO9" s="13">
         <v>6</v>
       </c>
-      <c r="AN9">
+      <c r="AP9">
         <v>70000</v>
       </c>
-      <c r="AO9">
+      <c r="AQ9">
         <v>7</v>
       </c>
-      <c r="AP9">
+      <c r="AR9">
         <v>0.90902324333846707</v>
       </c>
-      <c r="AQ9">
+      <c r="AS9">
         <v>3.890673718202788</v>
       </c>
-      <c r="AR9">
+      <c r="AT9">
         <v>2.2251599999999998</v>
       </c>
-      <c r="AT9">
+      <c r="AV9">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV9" s="14">
+      <c r="AX9" s="13">
         <v>6</v>
       </c>
-      <c r="AW9">
+      <c r="AY9">
         <v>25000</v>
       </c>
-      <c r="AX9">
+      <c r="AZ9">
         <v>7</v>
       </c>
-      <c r="AY9">
+      <c r="BA9">
         <v>0.51339599194252106</v>
       </c>
-      <c r="AZ9">
+      <c r="BB9">
         <v>2.8635889594376751</v>
       </c>
-      <c r="BA9">
+      <c r="BC9">
         <v>1.5974999999999999</v>
       </c>
-      <c r="BC9">
+      <c r="BE9">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG9" s="13">
+        <v>6</v>
+      </c>
+      <c r="BH9">
+        <v>22500</v>
+      </c>
+      <c r="BI9">
+        <v>7</v>
+      </c>
+      <c r="BJ9">
+        <v>0.61575704291743538</v>
+      </c>
+      <c r="BK9">
+        <v>4.2136151266939219</v>
+      </c>
+      <c r="BL9">
+        <v>3.226999999999999</v>
+      </c>
+      <c r="BN9">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>7</v>
       </c>
@@ -1645,113 +1821,134 @@
       <c r="H10">
         <v>2.995599830918374</v>
       </c>
-      <c r="L10" s="2">
+      <c r="N10" s="2">
         <v>7</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>50000</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>8</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>1.0057722220136109</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>3.5998258948558881</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>2.48062</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U10" s="13">
+      <c r="W10" s="13">
         <v>7</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>75000</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <v>8</v>
       </c>
-      <c r="X10">
+      <c r="Z10">
         <v>0.9304421052752393</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <v>3.2725045109609678</v>
       </c>
-      <c r="Z10">
+      <c r="AB10">
         <v>2.3569</v>
       </c>
-      <c r="AB10">
+      <c r="AD10">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD10" s="13">
+      <c r="AF10" s="13">
         <v>7</v>
       </c>
-      <c r="AE10">
+      <c r="AG10">
         <v>90000</v>
       </c>
-      <c r="AF10">
+      <c r="AH10">
         <v>8</v>
       </c>
-      <c r="AG10">
+      <c r="AI10">
         <v>1.0781610172016991</v>
       </c>
-      <c r="AH10">
+      <c r="AJ10">
         <v>3.047668137060386</v>
       </c>
-      <c r="AI10">
+      <c r="AK10">
         <v>2.4780500000000001</v>
       </c>
-      <c r="AK10">
+      <c r="AM10">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM10" s="13">
+      <c r="AO10" s="13">
         <v>7</v>
       </c>
-      <c r="AN10">
+      <c r="AP10">
         <v>70000</v>
       </c>
-      <c r="AO10">
+      <c r="AQ10">
         <v>8</v>
       </c>
-      <c r="AP10">
+      <c r="AR10">
         <v>0.93068688369503749</v>
       </c>
-      <c r="AQ10">
+      <c r="AS10">
         <v>3.8851626912297319</v>
       </c>
-      <c r="AR10">
+      <c r="AT10">
         <v>2.2700900000000002</v>
       </c>
-      <c r="AT10">
+      <c r="AV10">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV10" s="14">
+      <c r="AX10" s="13">
         <v>7</v>
       </c>
-      <c r="AW10">
+      <c r="AY10">
         <v>25000</v>
       </c>
-      <c r="AX10">
+      <c r="AZ10">
         <v>8</v>
       </c>
-      <c r="AY10">
+      <c r="BA10">
         <v>0.51969332790896883</v>
       </c>
-      <c r="AZ10">
+      <c r="BB10">
         <v>2.8618594153307289</v>
       </c>
-      <c r="BA10">
+      <c r="BC10">
         <v>1.6208450000000001</v>
       </c>
-      <c r="BC10">
+      <c r="BE10">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG10" s="13">
+        <v>7</v>
+      </c>
+      <c r="BH10">
+        <v>22500</v>
+      </c>
+      <c r="BI10">
+        <v>8</v>
+      </c>
+      <c r="BJ10">
+        <v>0.63114500185174216</v>
+      </c>
+      <c r="BK10">
+        <v>4.2209504061763301</v>
+      </c>
+      <c r="BL10">
+        <v>3.2835000000000001</v>
+      </c>
+      <c r="BN10">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -1773,137 +1970,158 @@
       <c r="H11">
         <v>2.995599830918374</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N11" s="2">
         <v>8</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>50000</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>9</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>1.0108933166398251</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>3.5986832243048559</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>2.49329</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>3.7310623364769291</v>
       </c>
-      <c r="U11" s="13">
+      <c r="W11" s="13">
         <v>8</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>75000</v>
       </c>
-      <c r="W11">
+      <c r="Y11">
         <v>9</v>
       </c>
-      <c r="X11">
+      <c r="Z11">
         <v>0.93761111150821319</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <v>3.268319359703324</v>
       </c>
-      <c r="Z11">
+      <c r="AB11">
         <v>2.37229</v>
       </c>
-      <c r="AB11">
+      <c r="AD11">
         <v>3.748694078222786</v>
       </c>
-      <c r="AD11" s="13">
+      <c r="AF11" s="13">
         <v>8</v>
       </c>
-      <c r="AE11">
+      <c r="AG11">
         <v>90000</v>
       </c>
-      <c r="AF11">
+      <c r="AH11">
         <v>9</v>
       </c>
-      <c r="AG11">
+      <c r="AI11">
         <v>1.0843492319356911</v>
       </c>
-      <c r="AH11">
+      <c r="AJ11">
         <v>3.0469519551982178</v>
       </c>
-      <c r="AI11">
+      <c r="AK11">
         <v>2.4956499999999999</v>
       </c>
-      <c r="AK11">
+      <c r="AM11">
         <v>3.68572083840303</v>
       </c>
-      <c r="AM11" s="13">
+      <c r="AO11" s="13">
         <v>8</v>
       </c>
-      <c r="AN11">
+      <c r="AP11">
         <v>70000</v>
       </c>
-      <c r="AO11">
+      <c r="AQ11">
         <v>9</v>
       </c>
-      <c r="AP11">
+      <c r="AR11">
         <v>0.93225341578754384</v>
       </c>
-      <c r="AQ11">
+      <c r="AS11">
         <v>3.8853954153393269</v>
       </c>
-      <c r="AR11">
+      <c r="AT11">
         <v>2.2775379999999998</v>
       </c>
-      <c r="AT11">
+      <c r="AV11">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AV11" s="14">
+      <c r="AX11" s="13">
         <v>8</v>
       </c>
-      <c r="AW11">
+      <c r="AY11">
         <v>25000</v>
       </c>
-      <c r="AX11">
+      <c r="AZ11">
         <v>9</v>
       </c>
-      <c r="AY11">
+      <c r="BA11">
         <v>0.52078218128686538</v>
       </c>
-      <c r="AZ11">
+      <c r="BB11">
         <v>2.8626624943766159</v>
       </c>
-      <c r="BA11">
+      <c r="BC11">
         <v>1.629678</v>
       </c>
-      <c r="BC11">
+      <c r="BE11">
         <v>3.226396680182666</v>
       </c>
+      <c r="BG11" s="13">
+        <v>8</v>
+      </c>
+      <c r="BH11">
+        <v>22500</v>
+      </c>
+      <c r="BI11">
+        <v>9</v>
+      </c>
+      <c r="BJ11">
+        <v>0.63329750718907252</v>
+      </c>
+      <c r="BK11">
+        <v>4.2253186197428194</v>
+      </c>
+      <c r="BL11">
+        <v>3.30043</v>
+      </c>
+      <c r="BN11">
+        <v>4.0476445154746212</v>
+      </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="L13" s="11"/>
+      <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="N15" s="3"/>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>1</v>
       </c>
@@ -1925,26 +2143,29 @@
       <c r="H18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" s="5" t="s">
+      <c r="I18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="Q18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P18" s="5" t="s">
+      <c r="R18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Q18" s="5" t="s">
+      <c r="S18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="T18" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>1</v>
       </c>
@@ -1966,13 +2187,10 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="M19" s="6">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19">
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="O19" s="6">
         <v>1</v>
       </c>
       <c r="P19">
@@ -1984,8 +2202,14 @@
       <c r="R19">
         <v>1</v>
       </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <f>B19+1</f>
         <v>2</v>
@@ -1995,51 +2219,55 @@
         <v>6.3247996944086865E-2</v>
       </c>
       <c r="D20" s="4">
-        <f>(P3-P4)/P4</f>
+        <f>(R3-R4)/R4</f>
         <v>3.3949119828678542E-2</v>
       </c>
       <c r="E20" s="4">
-        <f>(Y3-Y4)/Y4</f>
+        <f>(AA3-AA4)/AA4</f>
         <v>7.1026924660783808E-2</v>
       </c>
       <c r="F20">
-        <f>(AH3-AH4)/AH4</f>
+        <f>(AJ3-AJ4)/AJ4</f>
         <v>4.6470246278268193E-2</v>
       </c>
       <c r="G20">
-        <f>(AQ3-AQ4)/AQ4</f>
+        <f>(AS3-AS4)/AS4</f>
         <v>1.1042853717827929E-2</v>
       </c>
       <c r="H20" s="7">
-        <f>(AZ3-AZ4)/AZ4</f>
+        <f>(BB3-BB4)/BB4</f>
         <v>1.6189398497926916E-2</v>
       </c>
-      <c r="M20" s="6">
-        <f>M19+1</f>
+      <c r="I20">
+        <f>(BK3-BK4)/BK4</f>
+        <v>1.8669803107859016E-2</v>
+      </c>
+      <c r="O20" s="6">
+        <f>O19+1</f>
         <v>2</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <f>(D4-D3)/D4</f>
         <v>0.39581363878321912</v>
       </c>
-      <c r="O20">
-        <f>(O4-O3)/O4</f>
+      <c r="Q20">
+        <f>(Q4-Q3)/Q4</f>
         <v>0.37183807205949732</v>
       </c>
-      <c r="P20">
-        <f>(X4-X3)/X4</f>
+      <c r="R20">
+        <f>(Z4-Z3)/Z4</f>
         <v>0.44886597259574035</v>
       </c>
-      <c r="Q20">
-        <f>(AG4-AG3)/AG4</f>
+      <c r="S20">
+        <f>(AI4-AI3)/AI4</f>
         <v>0.26120216127717649</v>
       </c>
-      <c r="R20">
-        <f>(AP4-AP3)/AP4</f>
+      <c r="T20">
+        <f>(AR4-AR3)/AR4</f>
         <v>0.25951198234371448</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <f t="shared" ref="B21:B28" si="0">B20+1</f>
         <v>3</v>
@@ -2049,51 +2277,55 @@
         <v>1.476470116554285E-2</v>
       </c>
       <c r="D21">
-        <f>(P4-P5)/P5</f>
+        <f>(R4-R5)/R5</f>
         <v>1.602522029832221E-3</v>
       </c>
       <c r="E21">
-        <f>(Y4-Y5)/Y5</f>
+        <f>(AA4-AA5)/AA5</f>
         <v>3.3893481774347456E-3</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F27" si="1">(AH4-AH5)/AH5</f>
+        <f t="shared" ref="F21:F27" si="1">(AJ4-AJ5)/AJ5</f>
         <v>2.6026202444045811E-3</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" ref="G21:G27" si="2">(AQ4-AQ5)/AQ5</f>
+        <f t="shared" ref="G21:G27" si="2">(AS4-AS5)/AS5</f>
         <v>2.0090557373475284E-2</v>
       </c>
       <c r="H21" s="4">
-        <f>(AZ4-AZ5)/AZ5</f>
+        <f>(BB4-BB5)/BB5</f>
         <v>1.6189914601774193E-2</v>
       </c>
-      <c r="M21" s="6">
-        <f t="shared" ref="M21:M28" si="3">M20+1</f>
+      <c r="I21">
+        <f t="shared" ref="I21:I27" si="3">(BK4-BK5)/BK5</f>
+        <v>-1.377665118715758E-2</v>
+      </c>
+      <c r="O21" s="6">
+        <f t="shared" ref="O21:O28" si="4">O20+1</f>
         <v>3</v>
       </c>
-      <c r="N21">
-        <f t="shared" ref="N21:N27" si="4">(D5-D4)/D5</f>
+      <c r="P21">
+        <f t="shared" ref="P21:P27" si="5">(D5-D4)/D5</f>
         <v>0.10176566872127661</v>
       </c>
-      <c r="O21">
-        <f t="shared" ref="O21:O29" si="5">(O5-O4)/O5</f>
+      <c r="Q21">
+        <f t="shared" ref="Q21:Q29" si="6">(Q5-Q4)/Q5</f>
         <v>8.5557354256765014E-2</v>
       </c>
-      <c r="P21">
-        <f t="shared" ref="P21:P27" si="6">(X5-X4)/X5</f>
+      <c r="R21">
+        <f t="shared" ref="R21:R27" si="7">(Z5-Z4)/Z5</f>
         <v>7.1481595096278494E-2</v>
       </c>
-      <c r="Q21">
-        <f t="shared" ref="Q21:Q27" si="7">(AG5-AG4)/AG5</f>
+      <c r="S21">
+        <f t="shared" ref="S21:S27" si="8">(AI5-AI4)/AI5</f>
         <v>9.773195075543345E-2</v>
       </c>
-      <c r="R21">
-        <f t="shared" ref="R21:R27" si="8">(AP5-AP4)/AP5</f>
+      <c r="T21">
+        <f t="shared" ref="T21:T27" si="9">(AR5-AR4)/AR5</f>
         <v>0.21229867917953107</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2103,11 +2335,11 @@
         <v>6.0519930267361223E-3</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" ref="D22:D27" si="9">(P5-P6)/P6</f>
+        <f t="shared" ref="D22:D27" si="10">(R5-R6)/R6</f>
         <v>9.1718676206817111E-4</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" ref="E22:E26" si="10">(Y5-Y6)/Y6</f>
+        <f t="shared" ref="E22:E26" si="11">(AA5-AA6)/AA6</f>
         <v>8.3788475357532057E-3</v>
       </c>
       <c r="F22" s="4">
@@ -2115,57 +2347,61 @@
         <v>2.6828585624238292E-2</v>
       </c>
       <c r="G22">
-        <f>(AQ5-AQ6)/AQ6</f>
+        <f>(AS5-AS6)/AS6</f>
         <v>-2.7003661730892947E-3</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H21:H27" si="11">(AZ5-AZ6)/AZ6</f>
+        <f t="shared" ref="H22:H27" si="12">(BB5-BB6)/BB6</f>
         <v>2.830162123108083E-3</v>
       </c>
-      <c r="M22" s="6">
+      <c r="I22">
         <f t="shared" si="3"/>
+        <v>7.9276243364072765E-3</v>
+      </c>
+      <c r="O22" s="6">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="N22" s="4">
-        <f t="shared" si="4"/>
+      <c r="P22" s="4">
+        <f t="shared" si="5"/>
         <v>7.6646158209822388E-2</v>
       </c>
-      <c r="O22" s="4">
-        <f t="shared" si="5"/>
+      <c r="Q22" s="4">
+        <f t="shared" si="6"/>
         <v>5.8682521593663856E-2</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="6"/>
+      <c r="R22">
+        <f t="shared" si="7"/>
         <v>7.2696141264064873E-2</v>
       </c>
-      <c r="Q22">
-        <f t="shared" si="7"/>
+      <c r="S22">
+        <f t="shared" si="8"/>
         <v>0.16708960155030728</v>
       </c>
-      <c r="R22" s="4">
-        <f t="shared" si="8"/>
+      <c r="T22" s="4">
+        <f t="shared" si="9"/>
         <v>5.9839952835964098E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:C27" si="12">(E6-E7)/E7</f>
+        <f t="shared" ref="C23:C27" si="13">(E6-E7)/E7</f>
         <v>1.2553697719539917E-3</v>
       </c>
       <c r="D23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2.8219906800217784E-3</v>
       </c>
       <c r="E23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.2751722261865736E-3</v>
       </c>
       <c r="F23" s="7">
-        <f>(AH6-AH7)/AH7</f>
+        <f>(AJ6-AJ7)/AJ7</f>
         <v>2.9653127752681885E-3</v>
       </c>
       <c r="G23">
@@ -2173,49 +2409,53 @@
         <v>9.7996902403431237E-3</v>
       </c>
       <c r="H23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3649289333831764E-3</v>
       </c>
-      <c r="M23" s="6">
+      <c r="I23">
         <f t="shared" si="3"/>
+        <v>-5.0952105195325526E-3</v>
+      </c>
+      <c r="O23" s="6">
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="N23">
-        <f t="shared" si="4"/>
+      <c r="P23">
+        <f t="shared" si="5"/>
         <v>4.9151504423963835E-2</v>
       </c>
-      <c r="O23">
-        <f t="shared" si="5"/>
+      <c r="Q23">
+        <f t="shared" si="6"/>
         <v>3.0016184734596496E-2</v>
       </c>
-      <c r="P23" s="4">
-        <f t="shared" si="6"/>
+      <c r="R23" s="4">
+        <f t="shared" si="7"/>
         <v>5.3218237177546097E-2</v>
       </c>
-      <c r="Q23" s="4">
-        <f t="shared" si="7"/>
+      <c r="S23" s="4">
+        <f t="shared" si="8"/>
         <v>3.899768779105587E-2</v>
       </c>
-      <c r="R23">
-        <f t="shared" si="8"/>
+      <c r="T23">
+        <f t="shared" si="9"/>
         <v>7.4313676922907565E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5.5331216924087842E-3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-6.4551222529511492E-4</v>
       </c>
       <c r="E24">
-        <f>(Y7-Y8)/Y8</f>
+        <f>(AA7-AA8)/AA8</f>
         <v>2.5626877884473687E-3</v>
       </c>
       <c r="F24">
@@ -2227,49 +2467,53 @@
         <v>-3.2183711518570545E-3</v>
       </c>
       <c r="H24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.8123563066437401E-3</v>
       </c>
-      <c r="M24" s="6">
+      <c r="I24">
         <f t="shared" si="3"/>
+        <v>-6.5248999949499781E-3</v>
+      </c>
+      <c r="O24" s="6">
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="N24">
-        <f t="shared" si="4"/>
+      <c r="P24">
+        <f t="shared" si="5"/>
         <v>4.2686815096649983E-2</v>
       </c>
-      <c r="O24">
-        <f t="shared" si="5"/>
+      <c r="Q24">
+        <f t="shared" si="6"/>
         <v>4.4278249967540102E-2</v>
       </c>
-      <c r="P24">
-        <f t="shared" si="6"/>
+      <c r="R24">
+        <f t="shared" si="7"/>
         <v>3.9822575755710674E-2</v>
       </c>
-      <c r="Q24">
-        <f t="shared" si="7"/>
+      <c r="S24">
+        <f t="shared" si="8"/>
         <v>1.8254949408081911E-2</v>
       </c>
-      <c r="R24">
-        <f t="shared" si="8"/>
+      <c r="T24">
+        <f t="shared" si="9"/>
         <v>2.620127547567833E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0474507201882914E-2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.8539505663454855E-3</v>
       </c>
       <c r="E25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>7.6313763388460958E-3</v>
       </c>
       <c r="F25">
@@ -2281,49 +2525,53 @@
         <v>-2.941055980213555E-3</v>
       </c>
       <c r="H25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.9029683520749106E-3</v>
       </c>
-      <c r="M25" s="6">
+      <c r="I25">
         <f t="shared" si="3"/>
+        <v>-2.8802283448994292E-3</v>
+      </c>
+      <c r="O25" s="6">
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="N25">
-        <f t="shared" si="4"/>
+      <c r="P25">
+        <f t="shared" si="5"/>
         <v>4.4785647777125841E-2</v>
       </c>
-      <c r="O25">
-        <f t="shared" si="5"/>
+      <c r="Q25">
+        <f t="shared" si="6"/>
         <v>3.4152860871484746E-2</v>
       </c>
-      <c r="P25">
-        <f t="shared" si="6"/>
+      <c r="R25">
+        <f t="shared" si="7"/>
         <v>3.8026372244194445E-2</v>
       </c>
-      <c r="Q25">
-        <f t="shared" si="7"/>
+      <c r="S25">
+        <f t="shared" si="8"/>
         <v>2.5035106576661761E-2</v>
       </c>
-      <c r="R25">
-        <f t="shared" si="8"/>
+      <c r="T25">
+        <f t="shared" si="9"/>
         <v>1.0543091480369964E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.0720710504481175E-3</v>
       </c>
       <c r="D26">
-        <f>(P9-P10)/P10</f>
+        <f>(R9-R10)/R10</f>
         <v>7.8479949475812312E-4</v>
       </c>
       <c r="E26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.32010104704502E-3</v>
       </c>
       <c r="F26">
@@ -2335,49 +2583,53 @@
         <v>1.4184803600365327E-3</v>
       </c>
       <c r="H26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6.0434279115222837E-4</v>
       </c>
-      <c r="M26" s="6">
+      <c r="I26">
         <f t="shared" si="3"/>
+        <v>-1.7378265026935181E-3</v>
+      </c>
+      <c r="O26" s="6">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="N26">
-        <f t="shared" si="4"/>
+      <c r="P26">
+        <f t="shared" si="5"/>
         <v>9.7504489348369978E-3</v>
       </c>
-      <c r="O26">
-        <f t="shared" si="5"/>
+      <c r="Q26">
+        <f t="shared" si="6"/>
         <v>1.2852928851536664E-2</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="6"/>
+      <c r="R26">
+        <f t="shared" si="7"/>
         <v>1.4997704246726501E-2</v>
       </c>
-      <c r="Q26">
-        <f t="shared" si="7"/>
+      <c r="S26">
+        <f t="shared" si="8"/>
         <v>2.3023925946269997E-2</v>
       </c>
-      <c r="R26">
-        <f t="shared" si="8"/>
+      <c r="T26">
+        <f t="shared" si="9"/>
         <v>2.3277044875244048E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.0028820484149271E-3</v>
       </c>
       <c r="D27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.1752462770683504E-4</v>
       </c>
       <c r="E27">
-        <f>(Y10-Y11)/Y11</f>
+        <f>(AA10-AA11)/AA11</f>
         <v>1.2805209029584394E-3</v>
       </c>
       <c r="F27">
@@ -2389,63 +2641,67 @@
         <v>-5.9897149380518581E-5</v>
       </c>
       <c r="H27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.8053570669424576E-4</v>
       </c>
-      <c r="M27" s="6">
+      <c r="I27">
         <f t="shared" si="3"/>
+        <v>-1.0338187387996761E-3</v>
+      </c>
+      <c r="O27" s="6">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="N27">
-        <f t="shared" si="4"/>
+      <c r="P27">
+        <f t="shared" si="5"/>
         <v>4.4282359502808418E-3</v>
       </c>
-      <c r="O27">
-        <f t="shared" si="5"/>
+      <c r="Q27">
+        <f t="shared" si="6"/>
         <v>5.0659100638200602E-3</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="6"/>
+      <c r="R27">
+        <f t="shared" si="7"/>
         <v>7.6460337820037638E-3</v>
       </c>
-      <c r="Q27">
-        <f t="shared" si="7"/>
+      <c r="S27">
+        <f t="shared" si="8"/>
         <v>5.7068466060010122E-3</v>
       </c>
-      <c r="R27">
-        <f t="shared" si="8"/>
+      <c r="T27">
+        <f t="shared" si="9"/>
         <v>1.6803715234263625E-3</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M28" s="6">
-        <f t="shared" si="3"/>
+      <c r="O28" s="6">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="O28" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q28" t="e">
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <f>B28+1</f>
         <v>11</v>
       </c>
-      <c r="M29" s="6">
-        <f>M28+1</f>
+      <c r="O29" s="6">
+        <f>O28+1</f>
         <v>11</v>
       </c>
-      <c r="O29" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q29" t="e">
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
QAPF map area 3b
-very small area, part of 3b
-only 12 points , rock type differs entirely from area 3a, probably due to low amount of datapoints and still large distance between them
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/error_budget.xlsx
+++ b/_INTERPOLATION/error_budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_INTERPOLATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F60A9F4-8DBA-466C-A4ED-8F64B0BBCDB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB96E4C-CB1E-402A-B8ED-FAFE29D9E2B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B30A4CA7-3C11-47FA-9AAE-51C8F55DE748}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="24">
   <si>
     <t>search_radius</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>area3a</t>
+  </si>
+  <si>
+    <t>area3b</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -236,6 +239,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671D0FF-6F7B-4180-8916-6B2747DEAF8E}">
-  <dimension ref="A2:BN30"/>
+  <dimension ref="A2:BP30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,34 +572,34 @@
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="12" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="12" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="12" customWidth="1"/>
+    <col min="16" max="16" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="12" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="12" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="12" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="9" t="s">
         <v>0</v>
@@ -620,149 +626,151 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="O2" s="1" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="Q2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="Y2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="Z2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="12" t="s">
+      <c r="AA2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AC2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AD2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AE2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AD2" s="12" t="s">
+      <c r="AF2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AH2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AG2" s="12" t="s">
+      <c r="AI2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AH2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="12" t="s">
+      <c r="AJ2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="12" t="s">
+      <c r="AL2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AK2" s="12" t="s">
+      <c r="AM2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AL2" s="12" t="s">
+      <c r="AN2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AM2" s="12" t="s">
+      <c r="AO2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AP2" s="12" t="s">
+      <c r="AR2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AQ2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="12" t="s">
+      <c r="AS2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AS2" s="12" t="s">
+      <c r="AU2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AT2" s="12" t="s">
+      <c r="AV2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AU2" s="12" t="s">
+      <c r="AW2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AV2" s="12" t="s">
+      <c r="AX2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AX2" s="14" t="s">
+      <c r="AZ2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AY2" s="12" t="s">
+      <c r="BA2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AZ2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA2" s="12" t="s">
+      <c r="BB2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="BB2" s="12" t="s">
+      <c r="BD2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="BC2" s="12" t="s">
+      <c r="BE2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="BD2" s="12" t="s">
+      <c r="BF2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="BE2" s="12" t="s">
+      <c r="BG2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="BG2" s="8" t="s">
+      <c r="BI2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="BH2" s="12" t="s">
+      <c r="BJ2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="BI2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="BJ2" s="12" t="s">
+      <c r="BK2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="BK2" s="12" t="s">
+      <c r="BM2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="BL2" s="12" t="s">
+      <c r="BN2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="BM2" s="12" t="s">
+      <c r="BO2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="BN2" s="12" t="s">
+      <c r="BP2" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
         <v>0</v>
       </c>
@@ -784,134 +792,134 @@
       <c r="H3">
         <v>2.995599830918374</v>
       </c>
-      <c r="N3" s="2">
+      <c r="P3" s="2">
         <v>0</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>50000</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
         <v>0.48067336594687038</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>3.7283063930572342</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>0.95240000000000002</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W3" s="13">
+      <c r="Y3" s="13">
         <v>0</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>75000</v>
       </c>
-      <c r="Y3">
-        <v>1</v>
-      </c>
-      <c r="Z3">
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
         <v>0.38033031902469272</v>
       </c>
-      <c r="AA3">
+      <c r="AC3">
         <v>3.6025795623284291</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>0.75180000000000002</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF3" s="13">
+      <c r="AH3" s="13">
         <v>0</v>
       </c>
-      <c r="AG3">
+      <c r="AI3">
         <v>90000</v>
       </c>
-      <c r="AH3">
-        <v>1</v>
-      </c>
-      <c r="AI3">
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
         <v>0.53794659513894327</v>
       </c>
-      <c r="AJ3">
+      <c r="AL3">
         <v>3.296988220851615</v>
       </c>
-      <c r="AK3">
+      <c r="AM3">
         <v>1.006</v>
       </c>
-      <c r="AM3">
+      <c r="AO3">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO3" s="13">
+      <c r="AQ3" s="13">
         <v>0</v>
       </c>
-      <c r="AP3">
+      <c r="AR3">
         <v>70000</v>
       </c>
-      <c r="AQ3">
-        <v>1</v>
-      </c>
-      <c r="AR3">
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
         <v>0.44461726443180999</v>
       </c>
-      <c r="AS3">
+      <c r="AU3">
         <v>4.0161955823321929</v>
       </c>
-      <c r="AT3">
+      <c r="AV3">
         <v>0.68979999999999997</v>
       </c>
-      <c r="AV3">
+      <c r="AX3">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX3" s="13">
+      <c r="AZ3" s="13">
         <v>0</v>
       </c>
-      <c r="AY3">
+      <c r="BA3">
         <v>25000</v>
       </c>
-      <c r="AZ3">
-        <v>1</v>
-      </c>
-      <c r="BA3">
+      <c r="BB3">
+        <v>1</v>
+      </c>
+      <c r="BC3">
         <v>0.3135243332821549</v>
       </c>
-      <c r="BB3">
+      <c r="BD3">
         <v>2.9954063794763091</v>
       </c>
-      <c r="BC3">
+      <c r="BE3">
         <v>0.70279999999999998</v>
       </c>
-      <c r="BE3">
+      <c r="BG3">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG3" s="13">
+      <c r="BI3" s="13">
         <v>0</v>
       </c>
-      <c r="BH3">
+      <c r="BJ3">
         <v>22500</v>
       </c>
-      <c r="BI3">
-        <v>1</v>
-      </c>
-      <c r="BJ3">
+      <c r="BK3">
+        <v>1</v>
+      </c>
+      <c r="BL3">
         <v>0.22445657144535569</v>
       </c>
-      <c r="BK3">
+      <c r="BM3">
         <v>4.2051235592021188</v>
       </c>
-      <c r="BL3">
+      <c r="BN3">
         <v>1.3351999999999999</v>
       </c>
-      <c r="BN3">
+      <c r="BP3">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -933,134 +941,134 @@
       <c r="H4">
         <v>2.995599830918374</v>
       </c>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4">
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <v>50000</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>2</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>0.76520614282182042</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>3.6058896144473729</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>1.4483999999999999</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W4" s="13">
-        <v>1</v>
-      </c>
-      <c r="X4">
+      <c r="Y4" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z4">
         <v>75000</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>2</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>0.69008680305220649</v>
       </c>
-      <c r="AA4">
+      <c r="AC4">
         <v>3.3636685309936909</v>
       </c>
-      <c r="AB4">
+      <c r="AD4">
         <v>1.3849</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF4" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG4">
+      <c r="AH4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI4">
         <v>90000</v>
       </c>
-      <c r="AH4">
+      <c r="AJ4">
         <v>2</v>
       </c>
-      <c r="AI4">
+      <c r="AK4">
         <v>0.72813774884466864</v>
       </c>
-      <c r="AJ4">
+      <c r="AL4">
         <v>3.1505799926727289</v>
       </c>
-      <c r="AK4">
+      <c r="AM4">
         <v>1.4530000000000001</v>
       </c>
-      <c r="AM4">
+      <c r="AO4">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO4" s="13">
-        <v>1</v>
-      </c>
-      <c r="AP4">
+      <c r="AQ4" s="13">
+        <v>1</v>
+      </c>
+      <c r="AR4">
         <v>70000</v>
       </c>
-      <c r="AQ4">
+      <c r="AS4">
         <v>2</v>
       </c>
-      <c r="AR4">
+      <c r="AT4">
         <v>0.60043816217184121</v>
       </c>
-      <c r="AS4">
+      <c r="AU4">
         <v>3.9723297262462758</v>
       </c>
-      <c r="AT4">
+      <c r="AV4">
         <v>1.1192</v>
       </c>
-      <c r="AV4">
+      <c r="AX4">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX4" s="13">
-        <v>1</v>
-      </c>
-      <c r="AY4">
+      <c r="AZ4" s="13">
+        <v>1</v>
+      </c>
+      <c r="BA4">
         <v>25000</v>
       </c>
-      <c r="AZ4">
+      <c r="BB4">
         <v>2</v>
       </c>
-      <c r="BA4">
+      <c r="BC4">
         <v>0.38298251998665372</v>
       </c>
-      <c r="BB4">
+      <c r="BD4">
         <v>2.9476851302561782</v>
       </c>
-      <c r="BC4">
+      <c r="BE4">
         <v>0.92720000000000002</v>
       </c>
-      <c r="BE4">
+      <c r="BG4">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG4" s="13">
-        <v>1</v>
-      </c>
-      <c r="BH4">
+      <c r="BI4" s="13">
+        <v>1</v>
+      </c>
+      <c r="BJ4">
         <v>22500</v>
       </c>
-      <c r="BI4">
+      <c r="BK4">
         <v>2</v>
       </c>
-      <c r="BJ4">
+      <c r="BL4">
         <v>0.36957190579716998</v>
       </c>
-      <c r="BK4">
+      <c r="BM4">
         <v>4.1280536110648516</v>
       </c>
-      <c r="BL4">
+      <c r="BN4">
         <v>1.8603000000000001</v>
       </c>
-      <c r="BN4">
+      <c r="BP4">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>2</v>
       </c>
@@ -1082,134 +1090,134 @@
       <c r="H5">
         <v>2.995599830918374</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>2</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>50000</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>3</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>0.83680058709409921</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>3.600120342288808</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>1.7071000000000001</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W5" s="13">
+      <c r="Y5" s="13">
         <v>2</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>75000</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>3</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>0.74321284253246644</v>
       </c>
-      <c r="AA5">
+      <c r="AC5">
         <v>3.3523063974154081</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>1.7165999999999999</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF5" s="13">
+      <c r="AH5" s="13">
         <v>2</v>
       </c>
-      <c r="AG5">
+      <c r="AI5">
         <v>90000</v>
       </c>
-      <c r="AH5">
+      <c r="AJ5">
         <v>3</v>
       </c>
-      <c r="AI5">
+      <c r="AK5">
         <v>0.80700823824395607</v>
       </c>
-      <c r="AJ5">
+      <c r="AL5">
         <v>3.14240151487407</v>
       </c>
-      <c r="AK5">
+      <c r="AM5">
         <v>1.7876000000000001</v>
       </c>
-      <c r="AM5">
+      <c r="AO5">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO5" s="13">
+      <c r="AQ5" s="13">
         <v>2</v>
       </c>
-      <c r="AP5">
+      <c r="AR5">
         <v>70000</v>
       </c>
-      <c r="AQ5">
+      <c r="AS5">
         <v>3</v>
       </c>
-      <c r="AR5">
+      <c r="AT5">
         <v>0.76226628837745936</v>
       </c>
-      <c r="AS5">
+      <c r="AU5">
         <v>3.8940951835435209</v>
       </c>
-      <c r="AT5">
+      <c r="AV5">
         <v>1.6471</v>
       </c>
-      <c r="AV5">
+      <c r="AX5">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX5" s="13">
+      <c r="AZ5" s="13">
         <v>2</v>
       </c>
-      <c r="AY5">
+      <c r="BA5">
         <v>25000</v>
       </c>
-      <c r="AZ5">
+      <c r="BB5">
         <v>3</v>
       </c>
-      <c r="BA5">
+      <c r="BC5">
         <v>0.44056957653022139</v>
       </c>
-      <c r="BB5">
+      <c r="BD5">
         <v>2.9007226778188611</v>
       </c>
-      <c r="BC5">
+      <c r="BE5">
         <v>1.1079399999999999</v>
       </c>
-      <c r="BE5">
+      <c r="BG5">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG5" s="13">
+      <c r="BI5" s="13">
         <v>2</v>
       </c>
-      <c r="BH5">
+      <c r="BJ5">
         <v>22500</v>
       </c>
-      <c r="BI5">
+      <c r="BK5">
         <v>3</v>
       </c>
-      <c r="BJ5">
+      <c r="BL5">
         <v>0.42531097324201539</v>
       </c>
-      <c r="BK5">
+      <c r="BM5">
         <v>4.1857187989251718</v>
       </c>
-      <c r="BL5">
+      <c r="BN5">
         <v>2.3582999999999998</v>
       </c>
-      <c r="BN5">
+      <c r="BP5">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -1231,134 +1239,134 @@
       <c r="H6">
         <v>2.995599830918374</v>
       </c>
-      <c r="N6" s="2">
+      <c r="P6" s="2">
         <v>3</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>50000</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>4</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>0.88896743796876532</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>3.5968213853286608</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>1.9228000000000001</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W6" s="13">
+      <c r="Y6" s="13">
         <v>3</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>75000</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>4</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <v>0.80147713775890628</v>
       </c>
-      <c r="AA6">
+      <c r="AC6">
         <v>3.3244513266097129</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <v>1.95</v>
       </c>
-      <c r="AD6">
+      <c r="AF6">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF6" s="13">
+      <c r="AH6" s="13">
         <v>3</v>
       </c>
-      <c r="AG6">
+      <c r="AI6">
         <v>90000</v>
       </c>
-      <c r="AH6">
+      <c r="AJ6">
         <v>4</v>
       </c>
-      <c r="AI6">
+      <c r="AK6">
         <v>0.96890162464780283</v>
       </c>
-      <c r="AJ6">
+      <c r="AL6">
         <v>3.0602980466926861</v>
       </c>
-      <c r="AK6">
+      <c r="AM6">
         <v>1.9857</v>
       </c>
-      <c r="AM6">
+      <c r="AO6">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO6" s="13">
+      <c r="AQ6" s="13">
         <v>3</v>
       </c>
-      <c r="AP6">
+      <c r="AR6">
         <v>70000</v>
       </c>
-      <c r="AQ6">
+      <c r="AS6">
         <v>4</v>
       </c>
-      <c r="AR6">
+      <c r="AT6">
         <v>0.81078353699118821</v>
       </c>
-      <c r="AS6">
+      <c r="AU6">
         <v>3.904639138992577</v>
       </c>
-      <c r="AT6">
+      <c r="AV6">
         <v>1.9302999999999999</v>
       </c>
-      <c r="AV6">
+      <c r="AX6">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX6" s="13">
+      <c r="AZ6" s="13">
         <v>3</v>
       </c>
-      <c r="AY6">
+      <c r="BA6">
         <v>25000</v>
       </c>
-      <c r="AZ6">
+      <c r="BB6">
         <v>4</v>
       </c>
-      <c r="BA6">
+      <c r="BC6">
         <v>0.46639236828656983</v>
       </c>
-      <c r="BB6">
+      <c r="BD6">
         <v>2.8925363310549952</v>
       </c>
-      <c r="BC6">
+      <c r="BE6">
         <v>1.30124</v>
       </c>
-      <c r="BE6">
+      <c r="BG6">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG6" s="13">
+      <c r="BI6" s="13">
         <v>3</v>
       </c>
-      <c r="BH6">
+      <c r="BJ6">
         <v>22500</v>
       </c>
-      <c r="BI6">
+      <c r="BK6">
         <v>4</v>
       </c>
-      <c r="BJ6">
+      <c r="BL6">
         <v>0.52555379164144767</v>
       </c>
-      <c r="BK6">
+      <c r="BM6">
         <v>4.1527969844867956</v>
       </c>
-      <c r="BL6">
+      <c r="BN6">
         <v>2.5823999999999998</v>
       </c>
-      <c r="BN6">
+      <c r="BP6">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>4</v>
       </c>
@@ -1380,134 +1388,134 @@
       <c r="H7">
         <v>2.995599830918374</v>
       </c>
-      <c r="N7" s="2">
+      <c r="P7" s="2">
         <v>4</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>50000</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>5</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>0.91647656793688792</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>3.6070003065766558</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>2.1351</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W7" s="13">
+      <c r="Y7" s="13">
         <v>4</v>
       </c>
-      <c r="X7">
+      <c r="Z7">
         <v>75000</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>5</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <v>0.84652785808803543</v>
       </c>
-      <c r="AA7">
+      <c r="AC7">
         <v>3.3135987201128718</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>2.0798000000000001</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF7" s="13">
+      <c r="AH7" s="13">
         <v>4</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>90000</v>
       </c>
-      <c r="AH7">
+      <c r="AJ7">
         <v>5</v>
       </c>
-      <c r="AI7">
+      <c r="AK7">
         <v>1.0082198682963639</v>
       </c>
-      <c r="AJ7">
+      <c r="AL7">
         <v>3.0512501356848012</v>
       </c>
-      <c r="AK7">
+      <c r="AM7">
         <v>2.1518999999999999</v>
       </c>
-      <c r="AM7">
+      <c r="AO7">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO7" s="13">
+      <c r="AQ7" s="13">
         <v>4</v>
       </c>
-      <c r="AP7">
+      <c r="AR7">
         <v>70000</v>
       </c>
-      <c r="AQ7">
+      <c r="AS7">
         <v>5</v>
       </c>
-      <c r="AR7">
+      <c r="AT7">
         <v>0.87587287051627427</v>
       </c>
-      <c r="AS7">
+      <c r="AU7">
         <v>3.8667462237616959</v>
       </c>
-      <c r="AT7">
+      <c r="AV7">
         <v>2.01986</v>
       </c>
-      <c r="AV7">
+      <c r="AX7">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX7" s="13">
+      <c r="AZ7" s="13">
         <v>4</v>
       </c>
-      <c r="AY7">
+      <c r="BA7">
         <v>25000</v>
       </c>
-      <c r="AZ7">
+      <c r="BB7">
         <v>5</v>
       </c>
-      <c r="BA7">
+      <c r="BC7">
         <v>0.48175799781117462</v>
       </c>
-      <c r="BB7">
+      <c r="BD7">
         <v>2.888593606065291</v>
       </c>
-      <c r="BC7">
+      <c r="BE7">
         <v>1.4191400000000001</v>
       </c>
-      <c r="BE7">
+      <c r="BG7">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG7" s="13">
+      <c r="BI7" s="13">
         <v>4</v>
       </c>
-      <c r="BH7">
+      <c r="BJ7">
         <v>22500</v>
       </c>
-      <c r="BI7">
+      <c r="BK7">
         <v>5</v>
       </c>
-      <c r="BJ7">
+      <c r="BL7">
         <v>0.56381355508322006</v>
       </c>
-      <c r="BK7">
+      <c r="BM7">
         <v>4.1740647229724948</v>
       </c>
-      <c r="BL7">
+      <c r="BN7">
         <v>2.8435000000000001</v>
       </c>
-      <c r="BN7">
+      <c r="BP7">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -1529,134 +1537,134 @@
       <c r="H8">
         <v>2.995599830918374</v>
       </c>
-      <c r="N8" s="2">
+      <c r="P8" s="2">
         <v>5</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>50000</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>6</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>0.95893660252658364</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>3.609330173328666</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>2.3302999999999998</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W8" s="13">
+      <c r="Y8" s="13">
         <v>5</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <v>75000</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <v>6</v>
       </c>
-      <c r="Z8">
+      <c r="AB8">
         <v>0.88163691075563233</v>
       </c>
-      <c r="AA8">
+      <c r="AC8">
         <v>3.3051287071358479</v>
       </c>
-      <c r="AB8">
+      <c r="AD8">
         <v>2.2050000000000001</v>
       </c>
-      <c r="AD8">
+      <c r="AF8">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF8" s="13">
+      <c r="AH8" s="13">
         <v>5</v>
       </c>
-      <c r="AG8">
+      <c r="AI8">
         <v>90000</v>
       </c>
-      <c r="AH8">
+      <c r="AJ8">
         <v>6</v>
       </c>
-      <c r="AI8">
+      <c r="AK8">
         <v>1.026967100764586</v>
       </c>
-      <c r="AJ8">
+      <c r="AL8">
         <v>3.0533007950275342</v>
       </c>
-      <c r="AK8">
+      <c r="AM8">
         <v>2.2700999999999998</v>
       </c>
-      <c r="AM8">
+      <c r="AO8">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO8" s="13">
+      <c r="AQ8" s="13">
         <v>5</v>
       </c>
-      <c r="AP8">
+      <c r="AR8">
         <v>70000</v>
       </c>
-      <c r="AQ8">
+      <c r="AS8">
         <v>6</v>
       </c>
-      <c r="AR8">
+      <c r="AT8">
         <v>0.899439328126167</v>
       </c>
-      <c r="AS8">
+      <c r="AU8">
         <v>3.8792310289968079</v>
       </c>
-      <c r="AT8">
+      <c r="AV8">
         <v>2.1240600000000001</v>
       </c>
-      <c r="AV8">
+      <c r="AX8">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX8" s="13">
+      <c r="AZ8" s="13">
         <v>5</v>
       </c>
-      <c r="AY8">
+      <c r="BA8">
         <v>25000</v>
       </c>
-      <c r="AZ8">
+      <c r="BB8">
         <v>6</v>
       </c>
-      <c r="BA8">
+      <c r="BC8">
         <v>0.49471381023515693</v>
       </c>
-      <c r="BB8">
+      <c r="BD8">
         <v>2.8804926344385868</v>
       </c>
-      <c r="BC8">
+      <c r="BE8">
         <v>1.54254</v>
       </c>
-      <c r="BE8">
+      <c r="BG8">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG8" s="13">
+      <c r="BI8" s="13">
         <v>5</v>
       </c>
-      <c r="BH8">
+      <c r="BJ8">
         <v>22500</v>
       </c>
-      <c r="BI8">
+      <c r="BK8">
         <v>6</v>
       </c>
-      <c r="BJ8">
+      <c r="BL8">
         <v>0.59448430017612008</v>
       </c>
-      <c r="BK8">
+      <c r="BM8">
         <v>4.2014789529715211</v>
       </c>
-      <c r="BL8">
+      <c r="BN8">
         <v>3.0501</v>
       </c>
-      <c r="BN8">
+      <c r="BP8">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>6</v>
       </c>
@@ -1678,134 +1686,134 @@
       <c r="H9">
         <v>2.995599830918374</v>
       </c>
-      <c r="N9" s="2">
+      <c r="P9" s="2">
         <v>6</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>50000</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>7</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>0.99284510320321806</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>3.6026510363993882</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>2.4392999999999998</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W9" s="13">
+      <c r="Y9" s="13">
         <v>6</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>75000</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>7</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>0.91648760976161969</v>
       </c>
-      <c r="AA9">
+      <c r="AC9">
         <v>3.2800970521033079</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>2.3134000000000001</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF9" s="13">
+      <c r="AH9" s="13">
         <v>6</v>
       </c>
-      <c r="AG9">
+      <c r="AI9">
         <v>90000</v>
       </c>
-      <c r="AH9">
+      <c r="AJ9">
         <v>7</v>
       </c>
-      <c r="AI9">
+      <c r="AK9">
         <v>1.053337517783492</v>
       </c>
-      <c r="AJ9">
+      <c r="AL9">
         <v>3.050403551110147</v>
       </c>
-      <c r="AK9">
+      <c r="AM9">
         <v>2.3786</v>
       </c>
-      <c r="AM9">
+      <c r="AO9">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO9" s="13">
+      <c r="AQ9" s="13">
         <v>6</v>
       </c>
-      <c r="AP9">
+      <c r="AR9">
         <v>70000</v>
       </c>
-      <c r="AQ9">
+      <c r="AS9">
         <v>7</v>
       </c>
-      <c r="AR9">
+      <c r="AT9">
         <v>0.90902324333846707</v>
       </c>
-      <c r="AS9">
+      <c r="AU9">
         <v>3.890673718202788</v>
       </c>
-      <c r="AT9">
+      <c r="AV9">
         <v>2.2251599999999998</v>
       </c>
-      <c r="AV9">
+      <c r="AX9">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX9" s="13">
+      <c r="AZ9" s="13">
         <v>6</v>
       </c>
-      <c r="AY9">
+      <c r="BA9">
         <v>25000</v>
       </c>
-      <c r="AZ9">
+      <c r="BB9">
         <v>7</v>
       </c>
-      <c r="BA9">
+      <c r="BC9">
         <v>0.51339599194252106</v>
       </c>
-      <c r="BB9">
+      <c r="BD9">
         <v>2.8635889594376751</v>
       </c>
-      <c r="BC9">
+      <c r="BE9">
         <v>1.5974999999999999</v>
       </c>
-      <c r="BE9">
+      <c r="BG9">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG9" s="13">
+      <c r="BI9" s="13">
         <v>6</v>
       </c>
-      <c r="BH9">
+      <c r="BJ9">
         <v>22500</v>
       </c>
-      <c r="BI9">
+      <c r="BK9">
         <v>7</v>
       </c>
-      <c r="BJ9">
+      <c r="BL9">
         <v>0.61575704291743538</v>
       </c>
-      <c r="BK9">
+      <c r="BM9">
         <v>4.2136151266939219</v>
       </c>
-      <c r="BL9">
+      <c r="BN9">
         <v>3.226999999999999</v>
       </c>
-      <c r="BN9">
+      <c r="BP9">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>7</v>
       </c>
@@ -1827,134 +1835,134 @@
       <c r="H10">
         <v>2.995599830918374</v>
       </c>
-      <c r="N10" s="2">
+      <c r="P10" s="2">
         <v>7</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>50000</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>8</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>1.0057722220136109</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>3.5998258948558881</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>2.48062</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W10" s="13">
+      <c r="Y10" s="13">
         <v>7</v>
       </c>
-      <c r="X10">
+      <c r="Z10">
         <v>75000</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <v>8</v>
       </c>
-      <c r="Z10">
+      <c r="AB10">
         <v>0.9304421052752393</v>
       </c>
-      <c r="AA10">
+      <c r="AC10">
         <v>3.2725045109609678</v>
       </c>
-      <c r="AB10">
+      <c r="AD10">
         <v>2.3569</v>
       </c>
-      <c r="AD10">
+      <c r="AF10">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF10" s="13">
+      <c r="AH10" s="13">
         <v>7</v>
       </c>
-      <c r="AG10">
+      <c r="AI10">
         <v>90000</v>
       </c>
-      <c r="AH10">
+      <c r="AJ10">
         <v>8</v>
       </c>
-      <c r="AI10">
+      <c r="AK10">
         <v>1.0781610172016991</v>
       </c>
-      <c r="AJ10">
+      <c r="AL10">
         <v>3.047668137060386</v>
       </c>
-      <c r="AK10">
+      <c r="AM10">
         <v>2.4780500000000001</v>
       </c>
-      <c r="AM10">
+      <c r="AO10">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO10" s="13">
+      <c r="AQ10" s="13">
         <v>7</v>
       </c>
-      <c r="AP10">
+      <c r="AR10">
         <v>70000</v>
       </c>
-      <c r="AQ10">
+      <c r="AS10">
         <v>8</v>
       </c>
-      <c r="AR10">
+      <c r="AT10">
         <v>0.93068688369503749</v>
       </c>
-      <c r="AS10">
+      <c r="AU10">
         <v>3.8851626912297319</v>
       </c>
-      <c r="AT10">
+      <c r="AV10">
         <v>2.2700900000000002</v>
       </c>
-      <c r="AV10">
+      <c r="AX10">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX10" s="13">
+      <c r="AZ10" s="13">
         <v>7</v>
       </c>
-      <c r="AY10">
+      <c r="BA10">
         <v>25000</v>
       </c>
-      <c r="AZ10">
+      <c r="BB10">
         <v>8</v>
       </c>
-      <c r="BA10">
+      <c r="BC10">
         <v>0.51969332790896883</v>
       </c>
-      <c r="BB10">
+      <c r="BD10">
         <v>2.8618594153307289</v>
       </c>
-      <c r="BC10">
+      <c r="BE10">
         <v>1.6208450000000001</v>
       </c>
-      <c r="BE10">
+      <c r="BG10">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG10" s="13">
+      <c r="BI10" s="13">
         <v>7</v>
       </c>
-      <c r="BH10">
+      <c r="BJ10">
         <v>22500</v>
       </c>
-      <c r="BI10">
+      <c r="BK10">
         <v>8</v>
       </c>
-      <c r="BJ10">
+      <c r="BL10">
         <v>0.63114500185174216</v>
       </c>
-      <c r="BK10">
+      <c r="BM10">
         <v>4.2209504061763301</v>
       </c>
-      <c r="BL10">
+      <c r="BN10">
         <v>3.2835000000000001</v>
       </c>
-      <c r="BN10">
+      <c r="BP10">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -1976,158 +1984,158 @@
       <c r="H11">
         <v>2.995599830918374</v>
       </c>
-      <c r="N11" s="2">
+      <c r="P11" s="2">
         <v>8</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>50000</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>9</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>1.0108933166398251</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>3.5986832243048559</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>2.49329</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <v>3.7310623364769291</v>
       </c>
-      <c r="W11" s="13">
+      <c r="Y11" s="13">
         <v>8</v>
       </c>
-      <c r="X11">
+      <c r="Z11">
         <v>75000</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <v>9</v>
       </c>
-      <c r="Z11">
+      <c r="AB11">
         <v>0.93761111150821319</v>
       </c>
-      <c r="AA11">
+      <c r="AC11">
         <v>3.268319359703324</v>
       </c>
-      <c r="AB11">
+      <c r="AD11">
         <v>2.37229</v>
       </c>
-      <c r="AD11">
+      <c r="AF11">
         <v>3.748694078222786</v>
       </c>
-      <c r="AF11" s="13">
+      <c r="AH11" s="13">
         <v>8</v>
       </c>
-      <c r="AG11">
+      <c r="AI11">
         <v>90000</v>
       </c>
-      <c r="AH11">
+      <c r="AJ11">
         <v>9</v>
       </c>
-      <c r="AI11">
+      <c r="AK11">
         <v>1.0843492319356911</v>
       </c>
-      <c r="AJ11">
+      <c r="AL11">
         <v>3.0469519551982178</v>
       </c>
-      <c r="AK11">
+      <c r="AM11">
         <v>2.4956499999999999</v>
       </c>
-      <c r="AM11">
+      <c r="AO11">
         <v>3.68572083840303</v>
       </c>
-      <c r="AO11" s="13">
+      <c r="AQ11" s="13">
         <v>8</v>
       </c>
-      <c r="AP11">
+      <c r="AR11">
         <v>70000</v>
       </c>
-      <c r="AQ11">
+      <c r="AS11">
         <v>9</v>
       </c>
-      <c r="AR11">
+      <c r="AT11">
         <v>0.93225341578754384</v>
       </c>
-      <c r="AS11">
+      <c r="AU11">
         <v>3.8853954153393269</v>
       </c>
-      <c r="AT11">
+      <c r="AV11">
         <v>2.2775379999999998</v>
       </c>
-      <c r="AV11">
+      <c r="AX11">
         <v>4.1615592847749499</v>
       </c>
-      <c r="AX11" s="13">
+      <c r="AZ11" s="13">
         <v>8</v>
       </c>
-      <c r="AY11">
+      <c r="BA11">
         <v>25000</v>
       </c>
-      <c r="AZ11">
+      <c r="BB11">
         <v>9</v>
       </c>
-      <c r="BA11">
+      <c r="BC11">
         <v>0.52078218128686538</v>
       </c>
-      <c r="BB11">
+      <c r="BD11">
         <v>2.8626624943766159</v>
       </c>
-      <c r="BC11">
+      <c r="BE11">
         <v>1.629678</v>
       </c>
-      <c r="BE11">
+      <c r="BG11">
         <v>3.226396680182666</v>
       </c>
-      <c r="BG11" s="13">
+      <c r="BI11" s="13">
         <v>8</v>
       </c>
-      <c r="BH11">
+      <c r="BJ11">
         <v>22500</v>
       </c>
-      <c r="BI11">
+      <c r="BK11">
         <v>9</v>
       </c>
-      <c r="BJ11">
+      <c r="BL11">
         <v>0.63329750718907252</v>
       </c>
-      <c r="BK11">
+      <c r="BM11">
         <v>4.2253186197428194</v>
       </c>
-      <c r="BL11">
+      <c r="BN11">
         <v>3.30043</v>
       </c>
-      <c r="BN11">
+      <c r="BP11">
         <v>4.0476445154746212</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
-      <c r="N12" s="11"/>
+      <c r="P12" s="11"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="P13" s="11"/>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
-      <c r="N14" s="11"/>
+      <c r="P14" s="11"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="P15" s="3"/>
     </row>
-    <row r="17" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="O17" t="s">
+      <c r="Q17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>1</v>
       </c>
@@ -2155,50 +2163,75 @@
       <c r="J18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O18" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="P18" s="5" t="s">
+      <c r="K18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="5"/>
+      <c r="Q18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="Q18" s="5" t="s">
+      <c r="S18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="T18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="S18" s="5" t="s">
+      <c r="U18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="T18" s="5" t="s">
+      <c r="V18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AF18" s="8" t="s">
+      <c r="AH18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AG18" s="12" t="s">
+      <c r="AI18" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AH18" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI18" s="12" t="s">
+      <c r="AJ18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK18" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AJ18" s="12" t="s">
+      <c r="AL18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AK18" s="12" t="s">
+      <c r="AM18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AL18" s="12" t="s">
+      <c r="AN18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AM18" s="12" t="s">
+      <c r="AO18" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="AR18" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT18" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="AU18" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV18" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX18" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>1</v>
       </c>
@@ -2226,13 +2259,11 @@
       <c r="J19" s="7">
         <v>1</v>
       </c>
-      <c r="O19" s="6">
-        <v>1</v>
-      </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
-      <c r="Q19">
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="Q19" s="6">
         <v>1</v>
       </c>
       <c r="R19">
@@ -2244,29 +2275,56 @@
       <c r="T19">
         <v>1</v>
       </c>
-      <c r="AF19" s="13">
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="AH19" s="13">
         <v>0</v>
       </c>
-      <c r="AG19">
+      <c r="AI19">
         <v>14000</v>
       </c>
-      <c r="AH19">
-        <v>1</v>
-      </c>
-      <c r="AI19">
+      <c r="AJ19">
+        <v>1</v>
+      </c>
+      <c r="AK19">
         <v>0.31422856936735127</v>
       </c>
-      <c r="AJ19">
+      <c r="AL19">
         <v>2.054841055749284</v>
       </c>
-      <c r="AK19">
+      <c r="AM19">
         <v>0.84230000000000005</v>
       </c>
-      <c r="AM19">
+      <c r="AO19">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ19" s="15">
+        <v>0</v>
+      </c>
+      <c r="AR19">
+        <v>14000</v>
+      </c>
+      <c r="AS19">
+        <v>1</v>
+      </c>
+      <c r="AT19">
+        <v>1.6513097691810169E-2</v>
+      </c>
+      <c r="AU19">
+        <v>0.88823239422435396</v>
+      </c>
+      <c r="AV19">
+        <v>0.39150000000000001</v>
+      </c>
+      <c r="AX19">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <f>B19+1</f>
         <v>2</v>
@@ -2276,80 +2334,106 @@
         <v>6.3247996944086865E-2</v>
       </c>
       <c r="D20" s="4">
-        <f>(R3-R4)/R4</f>
+        <f>(T3-T4)/T4</f>
         <v>3.3949119828678542E-2</v>
       </c>
       <c r="E20" s="4">
-        <f>(AA3-AA4)/AA4</f>
+        <f>(AC3-AC4)/AC4</f>
         <v>7.1026924660783808E-2</v>
       </c>
       <c r="F20">
-        <f>(AJ3-AJ4)/AJ4</f>
+        <f>(AL3-AL4)/AL4</f>
         <v>4.6470246278268193E-2</v>
       </c>
       <c r="G20">
-        <f>(AS3-AS4)/AS4</f>
+        <f>(AU3-AU4)/AU4</f>
         <v>1.1042853717827929E-2</v>
       </c>
       <c r="H20" s="7">
-        <f>(BB3-BB4)/BB4</f>
+        <f>(BD3-BD4)/BD4</f>
         <v>1.6189398497926916E-2</v>
       </c>
       <c r="I20" s="4">
-        <f>(BK3-BK4)/BK4</f>
+        <f>(BM3-BM4)/BM4</f>
         <v>1.8669803107859016E-2</v>
       </c>
       <c r="J20" s="4">
-        <f>(AJ19-AJ20)/AJ20</f>
+        <f>(AL19-AL20)/AL20</f>
         <v>3.5312532254588018E-2</v>
       </c>
-      <c r="O20" s="6">
-        <f>O19+1</f>
+      <c r="K20" s="7">
+        <f>(AU19-AU20)/AU20</f>
+        <v>-8.0637663947796159E-2</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="Q20" s="6">
+        <f>Q19+1</f>
         <v>2</v>
       </c>
-      <c r="P20">
+      <c r="R20">
         <f>(D4-D3)/D4</f>
         <v>0.39581363878321912</v>
       </c>
-      <c r="Q20">
-        <f>(Q4-Q3)/Q4</f>
+      <c r="S20">
+        <f>(S4-S3)/S4</f>
         <v>0.37183807205949732</v>
       </c>
-      <c r="R20">
-        <f>(Z4-Z3)/Z4</f>
+      <c r="T20">
+        <f>(AB4-AB3)/AB4</f>
         <v>0.44886597259574035</v>
       </c>
-      <c r="S20">
-        <f>(AI4-AI3)/AI4</f>
+      <c r="U20">
+        <f>(AK4-AK3)/AK4</f>
         <v>0.26120216127717649</v>
       </c>
-      <c r="T20">
-        <f>(AR4-AR3)/AR4</f>
+      <c r="V20">
+        <f>(AT4-AT3)/AT4</f>
         <v>0.25951198234371448</v>
       </c>
-      <c r="AF20" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG20">
+      <c r="AH20" s="13">
+        <v>1</v>
+      </c>
+      <c r="AI20">
         <v>14000</v>
       </c>
-      <c r="AH20">
+      <c r="AJ20">
         <v>2</v>
       </c>
-      <c r="AI20">
+      <c r="AK20">
         <v>0.43663630326231812</v>
       </c>
-      <c r="AJ20">
+      <c r="AL20">
         <v>1.9847543536196559</v>
       </c>
-      <c r="AK20">
+      <c r="AM20">
         <v>1.2202</v>
       </c>
-      <c r="AM20">
+      <c r="AO20">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ20" s="15">
+        <v>1</v>
+      </c>
+      <c r="AR20">
+        <v>14000</v>
+      </c>
+      <c r="AS20">
+        <v>2</v>
+      </c>
+      <c r="AT20">
+        <v>2.280744337298005E-2</v>
+      </c>
+      <c r="AU20">
+        <v>0.96613963765197985</v>
+      </c>
+      <c r="AV20">
+        <v>0.50850000000000006</v>
+      </c>
+      <c r="AX20">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="21" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <f t="shared" ref="B21:B28" si="0">B20+1</f>
         <v>3</v>
@@ -2359,80 +2443,106 @@
         <v>1.476470116554285E-2</v>
       </c>
       <c r="D21">
-        <f>(R4-R5)/R5</f>
+        <f>(T4-T5)/T5</f>
         <v>1.602522029832221E-3</v>
       </c>
       <c r="E21">
-        <f>(AA4-AA5)/AA5</f>
+        <f>(AC4-AC5)/AC5</f>
         <v>3.3893481774347456E-3</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F27" si="1">(AJ4-AJ5)/AJ5</f>
+        <f t="shared" ref="F21:F27" si="1">(AL4-AL5)/AL5</f>
         <v>2.6026202444045811E-3</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" ref="G21:G27" si="2">(AS4-AS5)/AS5</f>
+        <f t="shared" ref="G21:G27" si="2">(AU4-AU5)/AU5</f>
         <v>2.0090557373475284E-2</v>
       </c>
       <c r="H21" s="4">
-        <f>(BB4-BB5)/BB5</f>
+        <f>(BD4-BD5)/BD5</f>
         <v>1.6189914601774193E-2</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:I27" si="3">(BK4-BK5)/BK5</f>
+        <f t="shared" ref="I21:I27" si="3">(BM4-BM5)/BM5</f>
         <v>-1.377665118715758E-2</v>
       </c>
       <c r="J21" s="7">
-        <f t="shared" ref="J21:J27" si="4">(AJ20-AJ21)/AJ21</f>
+        <f t="shared" ref="J21:J27" si="4">(AL20-AL21)/AL21</f>
         <v>-2.1916758437596592E-2</v>
       </c>
-      <c r="O21" s="6">
-        <f t="shared" ref="O21:O28" si="5">O20+1</f>
+      <c r="K21" s="7">
+        <f t="shared" ref="K21:K27" si="5">(AU20-AU21)/AU21</f>
+        <v>2.475683914293628E-2</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="Q21" s="6">
+        <f t="shared" ref="Q21:Q28" si="6">Q20+1</f>
         <v>3</v>
       </c>
-      <c r="P21">
-        <f t="shared" ref="P21:P27" si="6">(D5-D4)/D5</f>
+      <c r="R21">
+        <f t="shared" ref="R21:R27" si="7">(D5-D4)/D5</f>
         <v>0.10176566872127661</v>
       </c>
-      <c r="Q21">
-        <f t="shared" ref="Q21:Q29" si="7">(Q5-Q4)/Q5</f>
+      <c r="S21">
+        <f t="shared" ref="S21:S29" si="8">(S5-S4)/S5</f>
         <v>8.5557354256765014E-2</v>
       </c>
-      <c r="R21">
-        <f t="shared" ref="R21:R27" si="8">(Z5-Z4)/Z5</f>
+      <c r="T21">
+        <f t="shared" ref="T21:T27" si="9">(AB5-AB4)/AB5</f>
         <v>7.1481595096278494E-2</v>
       </c>
-      <c r="S21">
-        <f t="shared" ref="S21:S27" si="9">(AI5-AI4)/AI5</f>
+      <c r="U21">
+        <f t="shared" ref="U21:U27" si="10">(AK5-AK4)/AK5</f>
         <v>9.773195075543345E-2</v>
       </c>
-      <c r="T21">
-        <f t="shared" ref="T21:T27" si="10">(AR5-AR4)/AR5</f>
+      <c r="V21">
+        <f t="shared" ref="V21:V27" si="11">(AT5-AT4)/AT5</f>
         <v>0.21229867917953107</v>
       </c>
-      <c r="AF21" s="13">
+      <c r="AH21" s="13">
         <v>2</v>
       </c>
-      <c r="AG21">
+      <c r="AI21">
         <v>14000</v>
       </c>
-      <c r="AH21">
+      <c r="AJ21">
         <v>3</v>
       </c>
-      <c r="AI21">
+      <c r="AK21">
         <v>0.45510164011606169</v>
       </c>
-      <c r="AJ21">
+      <c r="AL21">
         <v>2.029228463672665</v>
       </c>
-      <c r="AK21">
+      <c r="AM21">
         <v>1.4260999999999999</v>
       </c>
-      <c r="AM21">
+      <c r="AO21">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ21" s="15">
+        <v>2</v>
+      </c>
+      <c r="AR21">
+        <v>14000</v>
+      </c>
+      <c r="AS21">
+        <v>3</v>
+      </c>
+      <c r="AT21">
+        <v>3.9652006835209863E-2</v>
+      </c>
+      <c r="AU21">
+        <v>0.94279891653128034</v>
+      </c>
+      <c r="AV21">
+        <v>0.59005000000000007</v>
+      </c>
+      <c r="AX21">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2442,11 +2552,11 @@
         <v>6.0519930267361223E-3</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" ref="D22:D27" si="11">(R5-R6)/R6</f>
+        <f t="shared" ref="D22:D27" si="12">(T5-T6)/T6</f>
         <v>9.1718676206817111E-4</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" ref="E22:E26" si="12">(AA5-AA6)/AA6</f>
+        <f t="shared" ref="E22:E26" si="13">(AC5-AC6)/AC6</f>
         <v>8.3788475357532057E-3</v>
       </c>
       <c r="F22" s="4">
@@ -2454,11 +2564,11 @@
         <v>2.6828585624238292E-2</v>
       </c>
       <c r="G22">
-        <f>(AS5-AS6)/AS6</f>
+        <f>(AU5-AU6)/AU6</f>
         <v>-2.7003661730892947E-3</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:H27" si="13">(BB5-BB6)/BB6</f>
+        <f t="shared" ref="H22:H27" si="14">(BD5-BD6)/BD6</f>
         <v>2.830162123108083E-3</v>
       </c>
       <c r="I22">
@@ -2469,71 +2579,97 @@
         <f t="shared" si="4"/>
         <v>-1.8350744816032227E-2</v>
       </c>
-      <c r="O22" s="6">
+      <c r="K22" s="7">
         <f t="shared" si="5"/>
+        <v>1.7906979263476507E-3</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="Q22" s="6">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="P22" s="4">
-        <f t="shared" si="6"/>
+      <c r="R22" s="4">
+        <f t="shared" si="7"/>
         <v>7.6646158209822388E-2</v>
       </c>
-      <c r="Q22" s="4">
-        <f t="shared" si="7"/>
+      <c r="S22" s="4">
+        <f t="shared" si="8"/>
         <v>5.8682521593663856E-2</v>
       </c>
-      <c r="R22">
-        <f t="shared" si="8"/>
+      <c r="T22">
+        <f t="shared" si="9"/>
         <v>7.2696141264064873E-2</v>
       </c>
-      <c r="S22">
-        <f t="shared" si="9"/>
+      <c r="U22">
+        <f t="shared" si="10"/>
         <v>0.16708960155030728</v>
       </c>
-      <c r="T22" s="4">
-        <f t="shared" si="10"/>
+      <c r="V22" s="4">
+        <f t="shared" si="11"/>
         <v>5.9839952835964098E-2</v>
       </c>
-      <c r="AF22" s="13">
+      <c r="AH22" s="13">
         <v>3</v>
       </c>
-      <c r="AG22">
+      <c r="AI22">
         <v>14000</v>
       </c>
-      <c r="AH22">
+      <c r="AJ22">
         <v>4</v>
       </c>
-      <c r="AI22">
+      <c r="AK22">
         <v>0.48008099093098472</v>
       </c>
-      <c r="AJ22">
+      <c r="AL22">
         <v>2.0671624339921428</v>
       </c>
-      <c r="AK22">
+      <c r="AM22">
         <v>1.5485</v>
       </c>
-      <c r="AM22">
+      <c r="AO22">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ22" s="15">
+        <v>3</v>
+      </c>
+      <c r="AR22">
+        <v>14000</v>
+      </c>
+      <c r="AS22">
+        <v>4</v>
+      </c>
+      <c r="AT22">
+        <v>5.4282398599628787E-2</v>
+      </c>
+      <c r="AU22">
+        <v>0.94111366624068571</v>
+      </c>
+      <c r="AV22">
+        <v>0.59388200000000002</v>
+      </c>
+      <c r="AX22">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:C27" si="14">(E6-E7)/E7</f>
+        <f t="shared" ref="C23:C27" si="15">(E6-E7)/E7</f>
         <v>1.2553697719539917E-3</v>
       </c>
       <c r="D23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-2.8219906800217784E-3</v>
       </c>
       <c r="E23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.2751722261865736E-3</v>
       </c>
       <c r="F23" s="7">
-        <f>(AJ6-AJ7)/AJ7</f>
+        <f>(AL6-AL7)/AL7</f>
         <v>2.9653127752681885E-3</v>
       </c>
       <c r="G23">
@@ -2541,7 +2677,7 @@
         <v>9.7996902403431237E-3</v>
       </c>
       <c r="H23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.3649289333831764E-3</v>
       </c>
       <c r="I23">
@@ -2552,67 +2688,93 @@
         <f t="shared" si="4"/>
         <v>1.2731287179369934E-3</v>
       </c>
-      <c r="O23" s="6">
+      <c r="K23" s="7">
         <f t="shared" si="5"/>
+        <v>-5.8982709138992355E-3</v>
+      </c>
+      <c r="L23" s="7"/>
+      <c r="Q23" s="6">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="6"/>
+      <c r="R23">
+        <f t="shared" si="7"/>
         <v>4.9151504423963835E-2</v>
       </c>
-      <c r="Q23">
-        <f t="shared" si="7"/>
+      <c r="S23">
+        <f t="shared" si="8"/>
         <v>3.0016184734596496E-2</v>
       </c>
-      <c r="R23" s="4">
-        <f t="shared" si="8"/>
+      <c r="T23" s="4">
+        <f t="shared" si="9"/>
         <v>5.3218237177546097E-2</v>
       </c>
-      <c r="S23" s="4">
-        <f t="shared" si="9"/>
+      <c r="U23" s="4">
+        <f t="shared" si="10"/>
         <v>3.899768779105587E-2</v>
       </c>
-      <c r="T23">
-        <f t="shared" si="10"/>
+      <c r="V23">
+        <f t="shared" si="11"/>
         <v>7.4313676922907565E-2</v>
       </c>
-      <c r="AF23" s="13">
+      <c r="AH23" s="13">
         <v>4</v>
       </c>
-      <c r="AG23">
+      <c r="AI23">
         <v>14000</v>
       </c>
-      <c r="AH23">
+      <c r="AJ23">
         <v>5</v>
       </c>
-      <c r="AI23">
+      <c r="AK23">
         <v>0.5226406867094312</v>
       </c>
-      <c r="AJ23">
+      <c r="AL23">
         <v>2.0645340164466468</v>
       </c>
-      <c r="AK23">
+      <c r="AM23">
         <v>1.6956</v>
       </c>
-      <c r="AM23">
+      <c r="AO23">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ23" s="15">
+        <v>4</v>
+      </c>
+      <c r="AR23">
+        <v>14000</v>
+      </c>
+      <c r="AS23">
+        <v>5</v>
+      </c>
+      <c r="AT23">
+        <v>5.8026462298956548E-2</v>
+      </c>
+      <c r="AU23">
+        <v>0.94669754483363777</v>
+      </c>
+      <c r="AV23">
+        <v>0.60322200000000004</v>
+      </c>
+      <c r="AX23">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.5331216924087842E-3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>-6.4551222529511492E-4</v>
       </c>
       <c r="E24">
-        <f>(AA7-AA8)/AA8</f>
+        <f>(AC7-AC8)/AC8</f>
         <v>2.5626877884473687E-3</v>
       </c>
       <c r="F24">
@@ -2624,7 +2786,7 @@
         <v>-3.2183711518570545E-3</v>
       </c>
       <c r="H24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.8123563066437401E-3</v>
       </c>
       <c r="I24">
@@ -2635,67 +2797,93 @@
         <f t="shared" si="4"/>
         <v>5.8531846459644226E-3</v>
       </c>
-      <c r="O24" s="6">
+      <c r="K24" s="7">
         <f t="shared" si="5"/>
+        <v>-4.5928708789333399E-3</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="Q24" s="6">
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="P24">
-        <f t="shared" si="6"/>
+      <c r="R24">
+        <f t="shared" si="7"/>
         <v>4.2686815096649983E-2</v>
       </c>
-      <c r="Q24">
-        <f t="shared" si="7"/>
+      <c r="S24">
+        <f t="shared" si="8"/>
         <v>4.4278249967540102E-2</v>
       </c>
-      <c r="R24">
-        <f t="shared" si="8"/>
+      <c r="T24">
+        <f t="shared" si="9"/>
         <v>3.9822575755710674E-2</v>
       </c>
-      <c r="S24">
-        <f t="shared" si="9"/>
+      <c r="U24">
+        <f t="shared" si="10"/>
         <v>1.8254949408081911E-2</v>
       </c>
-      <c r="T24">
-        <f t="shared" si="10"/>
+      <c r="V24">
+        <f t="shared" si="11"/>
         <v>2.620127547567833E-2</v>
       </c>
-      <c r="AF24" s="13">
+      <c r="AH24" s="13">
         <v>5</v>
       </c>
-      <c r="AG24">
+      <c r="AI24">
         <v>14000</v>
       </c>
-      <c r="AH24">
+      <c r="AJ24">
         <v>6</v>
       </c>
-      <c r="AI24">
+      <c r="AK24">
         <v>0.55026160561707127</v>
       </c>
-      <c r="AJ24">
+      <c r="AL24">
         <v>2.0525202365127591</v>
       </c>
-      <c r="AK24">
+      <c r="AM24">
         <v>1.7874000000000001</v>
       </c>
-      <c r="AM24">
+      <c r="AO24">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ24" s="15">
+        <v>5</v>
+      </c>
+      <c r="AR24">
+        <v>14000</v>
+      </c>
+      <c r="AS24">
+        <v>6</v>
+      </c>
+      <c r="AT24">
+        <v>5.8289543283584197E-2</v>
+      </c>
+      <c r="AU24">
+        <v>0.95106566663789227</v>
+      </c>
+      <c r="AV24">
+        <v>0.61840200000000001</v>
+      </c>
+      <c r="AX24">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.0474507201882914E-2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.8539505663454855E-3</v>
       </c>
       <c r="E25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7.6313763388460958E-3</v>
       </c>
       <c r="F25">
@@ -2707,7 +2895,7 @@
         <v>-2.941055980213555E-3</v>
       </c>
       <c r="H25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>5.9029683520749106E-3</v>
       </c>
       <c r="I25">
@@ -2718,67 +2906,93 @@
         <f t="shared" si="4"/>
         <v>-2.1010210922667262E-3</v>
       </c>
-      <c r="O25" s="6">
+      <c r="K25" s="7">
         <f t="shared" si="5"/>
+        <v>-7.3300212300288323E-4</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="Q25" s="6">
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="P25">
-        <f t="shared" si="6"/>
+      <c r="R25">
+        <f t="shared" si="7"/>
         <v>4.4785647777125841E-2</v>
       </c>
-      <c r="Q25">
-        <f t="shared" si="7"/>
+      <c r="S25">
+        <f t="shared" si="8"/>
         <v>3.4152860871484746E-2</v>
       </c>
-      <c r="R25">
-        <f t="shared" si="8"/>
+      <c r="T25">
+        <f t="shared" si="9"/>
         <v>3.8026372244194445E-2</v>
       </c>
-      <c r="S25">
-        <f t="shared" si="9"/>
+      <c r="U25">
+        <f t="shared" si="10"/>
         <v>2.5035106576661761E-2</v>
       </c>
-      <c r="T25">
-        <f t="shared" si="10"/>
+      <c r="V25">
+        <f t="shared" si="11"/>
         <v>1.0543091480369964E-2</v>
       </c>
-      <c r="AF25" s="13">
+      <c r="AH25" s="13">
         <v>6</v>
       </c>
-      <c r="AG25">
+      <c r="AI25">
         <v>14000</v>
       </c>
-      <c r="AH25">
+      <c r="AJ25">
         <v>7</v>
       </c>
-      <c r="AI25">
+      <c r="AK25">
         <v>0.55904622855672681</v>
       </c>
-      <c r="AJ25">
+      <c r="AL25">
         <v>2.0568417043169829</v>
       </c>
-      <c r="AK25">
+      <c r="AM25">
         <v>1.8151299999999999</v>
       </c>
-      <c r="AM25">
+      <c r="AO25">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ25" s="15">
+        <v>6</v>
+      </c>
+      <c r="AR25">
+        <v>14000</v>
+      </c>
+      <c r="AS25">
+        <v>7</v>
+      </c>
+      <c r="AT25">
+        <v>5.8329351121850267E-2</v>
+      </c>
+      <c r="AU25">
+        <v>0.95176331116557289</v>
+      </c>
+      <c r="AV25">
+        <v>0.62057600000000002</v>
+      </c>
+      <c r="AX25">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.0720710504481175E-3</v>
       </c>
       <c r="D26">
-        <f>(R9-R10)/R10</f>
+        <f>(T9-T10)/T10</f>
         <v>7.8479949475812312E-4</v>
       </c>
       <c r="E26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2.32010104704502E-3</v>
       </c>
       <c r="F26">
@@ -2790,7 +3004,7 @@
         <v>1.4184803600365327E-3</v>
       </c>
       <c r="H26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>6.0434279115222837E-4</v>
       </c>
       <c r="I26">
@@ -2801,67 +3015,93 @@
         <f t="shared" si="4"/>
         <v>-1.4576303322335088E-3</v>
       </c>
-      <c r="O26" s="6">
+      <c r="K26" s="7">
         <f t="shared" si="5"/>
+        <v>-2.4532980010266746E-4</v>
+      </c>
+      <c r="L26" s="7"/>
+      <c r="Q26" s="6">
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="6"/>
+      <c r="R26">
+        <f t="shared" si="7"/>
         <v>9.7504489348369978E-3</v>
       </c>
-      <c r="Q26">
-        <f t="shared" si="7"/>
+      <c r="S26">
+        <f t="shared" si="8"/>
         <v>1.2852928851536664E-2</v>
       </c>
-      <c r="R26">
-        <f t="shared" si="8"/>
+      <c r="T26">
+        <f t="shared" si="9"/>
         <v>1.4997704246726501E-2</v>
       </c>
-      <c r="S26">
-        <f t="shared" si="9"/>
+      <c r="U26">
+        <f t="shared" si="10"/>
         <v>2.3023925946269997E-2</v>
       </c>
-      <c r="T26">
-        <f t="shared" si="10"/>
+      <c r="V26">
+        <f t="shared" si="11"/>
         <v>2.3277044875244048E-2</v>
       </c>
-      <c r="AF26" s="13">
+      <c r="AH26" s="13">
         <v>7</v>
       </c>
-      <c r="AG26">
+      <c r="AI26">
         <v>14000</v>
       </c>
-      <c r="AH26">
+      <c r="AJ26">
         <v>8</v>
       </c>
-      <c r="AI26">
+      <c r="AK26">
         <v>0.56412695093570242</v>
       </c>
-      <c r="AJ26">
+      <c r="AL26">
         <v>2.0598441956963049</v>
       </c>
-      <c r="AK26">
+      <c r="AM26">
         <v>1.83718</v>
       </c>
-      <c r="AM26">
+      <c r="AO26">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ26" s="15">
+        <v>7</v>
+      </c>
+      <c r="AR26">
+        <v>14000</v>
+      </c>
+      <c r="AS26">
+        <v>8</v>
+      </c>
+      <c r="AT26">
+        <v>5.8340214444982483E-2</v>
+      </c>
+      <c r="AU26">
+        <v>0.95199686436600617</v>
+      </c>
+      <c r="AV26">
+        <v>0.62135200000000002</v>
+      </c>
+      <c r="AX26">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.0028820484149271E-3</v>
       </c>
       <c r="D27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3.1752462770683504E-4</v>
       </c>
       <c r="E27">
-        <f>(AA10-AA11)/AA11</f>
+        <f>(AC10-AC11)/AC11</f>
         <v>1.2805209029584394E-3</v>
       </c>
       <c r="F27">
@@ -2873,7 +3113,7 @@
         <v>-5.9897149380518581E-5</v>
       </c>
       <c r="H27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>-2.8053570669424576E-4</v>
       </c>
       <c r="I27">
@@ -2884,81 +3124,107 @@
         <f t="shared" si="4"/>
         <v>-1.1749029336880754E-3</v>
       </c>
-      <c r="O27" s="6">
+      <c r="K27" s="7">
         <f t="shared" si="5"/>
+        <v>-9.7588067995995947E-5</v>
+      </c>
+      <c r="L27" s="7"/>
+      <c r="Q27" s="6">
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="6"/>
+      <c r="R27">
+        <f t="shared" si="7"/>
         <v>4.4282359502808418E-3</v>
       </c>
-      <c r="Q27">
-        <f t="shared" si="7"/>
+      <c r="S27">
+        <f t="shared" si="8"/>
         <v>5.0659100638200602E-3</v>
       </c>
-      <c r="R27">
-        <f t="shared" si="8"/>
+      <c r="T27">
+        <f t="shared" si="9"/>
         <v>7.6460337820037638E-3</v>
       </c>
-      <c r="S27">
-        <f t="shared" si="9"/>
+      <c r="U27">
+        <f t="shared" si="10"/>
         <v>5.7068466060010122E-3</v>
       </c>
-      <c r="T27">
-        <f t="shared" si="10"/>
+      <c r="V27">
+        <f t="shared" si="11"/>
         <v>1.6803715234263625E-3</v>
       </c>
-      <c r="AF27" s="13">
+      <c r="AH27" s="13">
         <v>8</v>
       </c>
-      <c r="AG27">
+      <c r="AI27">
         <v>14000</v>
       </c>
-      <c r="AH27">
+      <c r="AJ27">
         <v>9</v>
       </c>
-      <c r="AI27">
+      <c r="AK27">
         <v>0.56534309497970381</v>
       </c>
-      <c r="AJ27">
+      <c r="AL27">
         <v>2.0622671594319701</v>
       </c>
-      <c r="AK27">
+      <c r="AM27">
         <v>1.8484799999999999</v>
       </c>
-      <c r="AM27">
+      <c r="AO27">
         <v>2.1509747809021862</v>
       </c>
+      <c r="AQ27" s="15">
+        <v>8</v>
+      </c>
+      <c r="AR27">
+        <v>14000</v>
+      </c>
+      <c r="AS27">
+        <v>9</v>
+      </c>
+      <c r="AT27">
+        <v>5.8349278038534548E-2</v>
+      </c>
+      <c r="AU27">
+        <v>0.9520897769678992</v>
+      </c>
+      <c r="AV27">
+        <v>0.62194400000000005</v>
+      </c>
+      <c r="AX27">
+        <v>0.83028189799088314</v>
+      </c>
     </row>
-    <row r="28" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O28" s="6">
-        <f t="shared" si="5"/>
+      <c r="Q28" s="6">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="Q28" t="e">
-        <f t="shared" si="7"/>
+      <c r="S28" t="e">
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <f>B28+1</f>
         <v>11</v>
       </c>
-      <c r="O29" s="6">
-        <f>O28+1</f>
+      <c r="Q29" s="6">
+        <f>Q28+1</f>
         <v>11</v>
       </c>
-      <c r="Q29" t="e">
-        <f t="shared" si="7"/>
+      <c r="S29" t="e">
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:50" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
QAPF map area 3c
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/error_budget.xlsx
+++ b/_INTERPOLATION/error_budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_INTERPOLATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB96E4C-CB1E-402A-B8ED-FAFE29D9E2B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F04D99-FB1B-4805-B9EA-8091AAADB233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B30A4CA7-3C11-47FA-9AAE-51C8F55DE748}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="27">
   <si>
     <t>search_radius</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>area3b</t>
+  </si>
+  <si>
+    <t>Area 3c</t>
+  </si>
+  <si>
+    <t>Area 3b</t>
+  </si>
+  <si>
+    <t>area 3c</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -239,9 +248,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -560,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671D0FF-6F7B-4180-8916-6B2747DEAF8E}">
   <dimension ref="A2:BP30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,7 +597,7 @@
     <col min="37" max="38" width="12" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="5" bestFit="1" customWidth="1"/>
     <col min="46" max="47" width="12" bestFit="1" customWidth="1"/>
@@ -2127,7 +2133,7 @@
       <c r="A15" s="3"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="17" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -2135,7 +2141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2172,9 @@
       <c r="K18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="Q18" s="5" t="s">
         <v>1</v>
       </c>
@@ -2209,29 +2217,56 @@
       <c r="AO18" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="AR18" s="15" t="s">
+      <c r="AQ18" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR18" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="AS18" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT18" s="15" t="s">
+      <c r="AS18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT18" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="AU18" s="15" t="s">
+      <c r="AU18" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AV18" s="15" t="s">
+      <c r="AV18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="AW18" s="15" t="s">
+      <c r="AW18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AX18" s="15" t="s">
+      <c r="AX18" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="AZ18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="BA18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC18" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="BE18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="BG18" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="19" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B19" s="6">
         <v>1</v>
       </c>
@@ -2262,7 +2297,9 @@
       <c r="K19" s="4">
         <v>1</v>
       </c>
-      <c r="L19" s="7"/>
+      <c r="L19" s="7">
+        <v>1</v>
+      </c>
       <c r="Q19" s="6">
         <v>1</v>
       </c>
@@ -2302,7 +2339,7 @@
       <c r="AO19">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ19" s="15">
+      <c r="AQ19" s="13">
         <v>0</v>
       </c>
       <c r="AR19">
@@ -2323,8 +2360,29 @@
       <c r="AX19">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ19" s="13">
+        <v>0</v>
+      </c>
+      <c r="BA19">
+        <v>20000</v>
+      </c>
+      <c r="BB19">
+        <v>1</v>
+      </c>
+      <c r="BC19">
+        <v>0.2112798674733572</v>
+      </c>
+      <c r="BD19">
+        <v>3.6981760732177049</v>
+      </c>
+      <c r="BE19">
+        <v>1.5298</v>
+      </c>
+      <c r="BG19">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="20" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <f>B19+1</f>
         <v>2</v>
@@ -2365,7 +2423,10 @@
         <f>(AU19-AU20)/AU20</f>
         <v>-8.0637663947796159E-2</v>
       </c>
-      <c r="L20" s="4"/>
+      <c r="L20" s="4">
+        <f>(BD19-BD20)/BD20</f>
+        <v>9.4632826092389807E-2</v>
+      </c>
       <c r="Q20" s="6">
         <f>Q19+1</f>
         <v>2</v>
@@ -2411,7 +2472,7 @@
       <c r="AO20">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ20" s="15">
+      <c r="AQ20" s="13">
         <v>1</v>
       </c>
       <c r="AR20">
@@ -2432,8 +2493,29 @@
       <c r="AX20">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ20" s="13">
+        <v>1</v>
+      </c>
+      <c r="BA20">
+        <v>20000</v>
+      </c>
+      <c r="BB20">
+        <v>2</v>
+      </c>
+      <c r="BC20">
+        <v>0.78896175297514703</v>
+      </c>
+      <c r="BD20">
+        <v>3.3784626087081819</v>
+      </c>
+      <c r="BE20">
+        <v>1.649</v>
+      </c>
+      <c r="BG20">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="21" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B21" s="6">
         <f t="shared" ref="B21:B28" si="0">B20+1</f>
         <v>3</v>
@@ -2474,29 +2556,32 @@
         <f t="shared" ref="K21:K27" si="5">(AU20-AU21)/AU21</f>
         <v>2.475683914293628E-2</v>
       </c>
-      <c r="L21" s="7"/>
+      <c r="L21" s="7">
+        <f t="shared" ref="L21:L27" si="6">(BD20-BD21)/BD21</f>
+        <v>-3.4941215570439897E-3</v>
+      </c>
       <c r="Q21" s="6">
-        <f t="shared" ref="Q21:Q28" si="6">Q20+1</f>
+        <f t="shared" ref="Q21:Q28" si="7">Q20+1</f>
         <v>3</v>
       </c>
       <c r="R21">
-        <f t="shared" ref="R21:R27" si="7">(D5-D4)/D5</f>
+        <f t="shared" ref="R21:R27" si="8">(D5-D4)/D5</f>
         <v>0.10176566872127661</v>
       </c>
       <c r="S21">
-        <f t="shared" ref="S21:S29" si="8">(S5-S4)/S5</f>
+        <f t="shared" ref="S21:S29" si="9">(S5-S4)/S5</f>
         <v>8.5557354256765014E-2</v>
       </c>
       <c r="T21">
-        <f t="shared" ref="T21:T27" si="9">(AB5-AB4)/AB5</f>
+        <f t="shared" ref="T21:T27" si="10">(AB5-AB4)/AB5</f>
         <v>7.1481595096278494E-2</v>
       </c>
       <c r="U21">
-        <f t="shared" ref="U21:U27" si="10">(AK5-AK4)/AK5</f>
+        <f t="shared" ref="U21:U27" si="11">(AK5-AK4)/AK5</f>
         <v>9.773195075543345E-2</v>
       </c>
       <c r="V21">
-        <f t="shared" ref="V21:V27" si="11">(AT5-AT4)/AT5</f>
+        <f t="shared" ref="V21:V27" si="12">(AT5-AT4)/AT5</f>
         <v>0.21229867917953107</v>
       </c>
       <c r="AH21" s="13">
@@ -2520,7 +2605,7 @@
       <c r="AO21">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ21" s="15">
+      <c r="AQ21" s="13">
         <v>2</v>
       </c>
       <c r="AR21">
@@ -2541,8 +2626,29 @@
       <c r="AX21">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ21" s="13">
+        <v>2</v>
+      </c>
+      <c r="BA21">
+        <v>20000</v>
+      </c>
+      <c r="BB21">
+        <v>3</v>
+      </c>
+      <c r="BC21">
+        <v>0.85624013185044456</v>
+      </c>
+      <c r="BD21">
+        <v>3.390308759630241</v>
+      </c>
+      <c r="BE21">
+        <v>1.67299</v>
+      </c>
+      <c r="BG21">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="22" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2552,11 +2658,11 @@
         <v>6.0519930267361223E-3</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" ref="D22:D27" si="12">(T5-T6)/T6</f>
+        <f t="shared" ref="D22:D27" si="13">(T5-T6)/T6</f>
         <v>9.1718676206817111E-4</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" ref="E22:E26" si="13">(AC5-AC6)/AC6</f>
+        <f t="shared" ref="E22:E26" si="14">(AC5-AC6)/AC6</f>
         <v>8.3788475357532057E-3</v>
       </c>
       <c r="F22" s="4">
@@ -2568,7 +2674,7 @@
         <v>-2.7003661730892947E-3</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:H27" si="14">(BD5-BD6)/BD6</f>
+        <f t="shared" ref="H22:H27" si="15">(BD5-BD6)/BD6</f>
         <v>2.830162123108083E-3</v>
       </c>
       <c r="I22">
@@ -2583,29 +2689,32 @@
         <f t="shared" si="5"/>
         <v>1.7906979263476507E-3</v>
       </c>
-      <c r="L22" s="7"/>
+      <c r="L22" s="7">
+        <f t="shared" si="6"/>
+        <v>2.4397135702748885E-3</v>
+      </c>
       <c r="Q22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="R22" s="4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.6646158209822388E-2</v>
       </c>
       <c r="S22" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.8682521593663856E-2</v>
       </c>
       <c r="T22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.2696141264064873E-2</v>
       </c>
       <c r="U22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.16708960155030728</v>
       </c>
       <c r="V22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.9839952835964098E-2</v>
       </c>
       <c r="AH22" s="13">
@@ -2629,7 +2738,7 @@
       <c r="AO22">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ22" s="15">
+      <c r="AQ22" s="13">
         <v>3</v>
       </c>
       <c r="AR22">
@@ -2650,22 +2759,43 @@
       <c r="AX22">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ22" s="13">
+        <v>3</v>
+      </c>
+      <c r="BA22">
+        <v>20000</v>
+      </c>
+      <c r="BB22">
+        <v>4</v>
+      </c>
+      <c r="BC22">
+        <v>0.90795121919934418</v>
+      </c>
+      <c r="BD22">
+        <v>3.3820575080324442</v>
+      </c>
+      <c r="BE22">
+        <v>1.7728900000000001</v>
+      </c>
+      <c r="BG22">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="23" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:C27" si="15">(E6-E7)/E7</f>
+        <f t="shared" ref="C23:C27" si="16">(E6-E7)/E7</f>
         <v>1.2553697719539917E-3</v>
       </c>
       <c r="D23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-2.8219906800217784E-3</v>
       </c>
       <c r="E23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>3.2751722261865736E-3</v>
       </c>
       <c r="F23" s="7">
@@ -2677,7 +2807,7 @@
         <v>9.7996902403431237E-3</v>
       </c>
       <c r="H23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3649289333831764E-3</v>
       </c>
       <c r="I23">
@@ -2692,29 +2822,32 @@
         <f t="shared" si="5"/>
         <v>-5.8982709138992355E-3</v>
       </c>
-      <c r="L23" s="7"/>
+      <c r="L23" s="7">
+        <f t="shared" si="6"/>
+        <v>-1.0375606843394333E-2</v>
+      </c>
       <c r="Q23" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="R23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.9151504423963835E-2</v>
       </c>
       <c r="S23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.0016184734596496E-2</v>
       </c>
       <c r="T23" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.3218237177546097E-2</v>
       </c>
       <c r="U23" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3.899768779105587E-2</v>
       </c>
       <c r="V23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7.4313676922907565E-2</v>
       </c>
       <c r="AH23" s="13">
@@ -2738,7 +2871,7 @@
       <c r="AO23">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ23" s="15">
+      <c r="AQ23" s="13">
         <v>4</v>
       </c>
       <c r="AR23">
@@ -2759,18 +2892,39 @@
       <c r="AX23">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ23" s="13">
+        <v>4</v>
+      </c>
+      <c r="BA23">
+        <v>20000</v>
+      </c>
+      <c r="BB23">
+        <v>5</v>
+      </c>
+      <c r="BC23">
+        <v>0.92721678724985468</v>
+      </c>
+      <c r="BD23">
+        <v>3.4175163136841169</v>
+      </c>
+      <c r="BE23">
+        <v>1.8817900000000001</v>
+      </c>
+      <c r="BG23">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="24" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.5331216924087842E-3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>-6.4551222529511492E-4</v>
       </c>
       <c r="E24">
@@ -2786,7 +2940,7 @@
         <v>-3.2183711518570545E-3</v>
       </c>
       <c r="H24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.8123563066437401E-3</v>
       </c>
       <c r="I24">
@@ -2801,29 +2955,32 @@
         <f t="shared" si="5"/>
         <v>-4.5928708789333399E-3</v>
       </c>
-      <c r="L24" s="7"/>
+      <c r="L24" s="7">
+        <f t="shared" si="6"/>
+        <v>-4.2272768298144952E-3</v>
+      </c>
       <c r="Q24" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="R24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.2686815096649983E-2</v>
       </c>
       <c r="S24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.4278249967540102E-2</v>
       </c>
       <c r="T24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.9822575755710674E-2</v>
       </c>
       <c r="U24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.8254949408081911E-2</v>
       </c>
       <c r="V24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.620127547567833E-2</v>
       </c>
       <c r="AH24" s="13">
@@ -2847,7 +3004,7 @@
       <c r="AO24">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ24" s="15">
+      <c r="AQ24" s="13">
         <v>5</v>
       </c>
       <c r="AR24">
@@ -2868,22 +3025,43 @@
       <c r="AX24">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ24" s="13">
+        <v>5</v>
+      </c>
+      <c r="BA24">
+        <v>20000</v>
+      </c>
+      <c r="BB24">
+        <v>6</v>
+      </c>
+      <c r="BC24">
+        <v>0.93248005872858164</v>
+      </c>
+      <c r="BD24">
+        <v>3.432024431040813</v>
+      </c>
+      <c r="BE24">
+        <v>1.90463</v>
+      </c>
+      <c r="BG24">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="25" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B25" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0474507201882914E-2</v>
       </c>
       <c r="D25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.8539505663454855E-3</v>
       </c>
       <c r="E25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>7.6313763388460958E-3</v>
       </c>
       <c r="F25">
@@ -2895,7 +3073,7 @@
         <v>-2.941055980213555E-3</v>
       </c>
       <c r="H25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.9029683520749106E-3</v>
       </c>
       <c r="I25">
@@ -2910,29 +3088,32 @@
         <f t="shared" si="5"/>
         <v>-7.3300212300288323E-4</v>
       </c>
-      <c r="L25" s="7"/>
+      <c r="L25" s="7">
+        <f t="shared" si="6"/>
+        <v>-1.1024116644161371E-3</v>
+      </c>
       <c r="Q25" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="R25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.4785647777125841E-2</v>
       </c>
       <c r="S25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.4152860871484746E-2</v>
       </c>
       <c r="T25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.8026372244194445E-2</v>
       </c>
       <c r="U25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.5035106576661761E-2</v>
       </c>
       <c r="V25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.0543091480369964E-2</v>
       </c>
       <c r="AH25" s="13">
@@ -2956,7 +3137,7 @@
       <c r="AO25">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ25" s="15">
+      <c r="AQ25" s="13">
         <v>6</v>
       </c>
       <c r="AR25">
@@ -2977,14 +3158,35 @@
       <c r="AX25">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ25" s="13">
+        <v>6</v>
+      </c>
+      <c r="BA25">
+        <v>20000</v>
+      </c>
+      <c r="BB25">
+        <v>7</v>
+      </c>
+      <c r="BC25">
+        <v>0.9374691948281535</v>
+      </c>
+      <c r="BD25">
+        <v>3.435812110388047</v>
+      </c>
+      <c r="BE25">
+        <v>1.92791</v>
+      </c>
+      <c r="BG25">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="26" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2.0720710504481175E-3</v>
       </c>
       <c r="D26">
@@ -2992,7 +3194,7 @@
         <v>7.8479949475812312E-4</v>
       </c>
       <c r="E26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>2.32010104704502E-3</v>
       </c>
       <c r="F26">
@@ -3004,7 +3206,7 @@
         <v>1.4184803600365327E-3</v>
       </c>
       <c r="H26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6.0434279115222837E-4</v>
       </c>
       <c r="I26">
@@ -3019,29 +3221,32 @@
         <f t="shared" si="5"/>
         <v>-2.4532980010266746E-4</v>
       </c>
-      <c r="L26" s="7"/>
+      <c r="L26" s="7">
+        <f t="shared" si="6"/>
+        <v>-6.6846274590690629E-5</v>
+      </c>
       <c r="Q26" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="R26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9.7504489348369978E-3</v>
       </c>
       <c r="S26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2852928851536664E-2</v>
       </c>
       <c r="T26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.4997704246726501E-2</v>
       </c>
       <c r="U26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.3023925946269997E-2</v>
       </c>
       <c r="V26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.3277044875244048E-2</v>
       </c>
       <c r="AH26" s="13">
@@ -3065,7 +3270,7 @@
       <c r="AO26">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ26" s="15">
+      <c r="AQ26" s="13">
         <v>7</v>
       </c>
       <c r="AR26">
@@ -3086,18 +3291,39 @@
       <c r="AX26">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ26" s="13">
+        <v>7</v>
+      </c>
+      <c r="BA26">
+        <v>20000</v>
+      </c>
+      <c r="BB26">
+        <v>8</v>
+      </c>
+      <c r="BC26">
+        <v>0.94016820150631564</v>
+      </c>
+      <c r="BD26">
+        <v>3.4360417969815131</v>
+      </c>
+      <c r="BE26">
+        <v>1.9418500000000001</v>
+      </c>
+      <c r="BG26">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="27" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0028820484149271E-3</v>
       </c>
       <c r="D27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3.1752462770683504E-4</v>
       </c>
       <c r="E27">
@@ -3113,7 +3339,7 @@
         <v>-5.9897149380518581E-5</v>
       </c>
       <c r="H27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-2.8053570669424576E-4</v>
       </c>
       <c r="I27">
@@ -3128,29 +3354,32 @@
         <f t="shared" si="5"/>
         <v>-9.7588067995995947E-5</v>
       </c>
-      <c r="L27" s="7"/>
+      <c r="L27" s="7">
+        <f t="shared" si="6"/>
+        <v>-2.1830652667643912E-4</v>
+      </c>
       <c r="Q27" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="R27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4.4282359502808418E-3</v>
       </c>
       <c r="S27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.0659100638200602E-3</v>
       </c>
       <c r="T27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7.6460337820037638E-3</v>
       </c>
       <c r="U27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.7068466060010122E-3</v>
       </c>
       <c r="V27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6803715234263625E-3</v>
       </c>
       <c r="AH27" s="13">
@@ -3174,7 +3403,7 @@
       <c r="AO27">
         <v>2.1509747809021862</v>
       </c>
-      <c r="AQ27" s="15">
+      <c r="AQ27" s="13">
         <v>8</v>
       </c>
       <c r="AR27">
@@ -3195,22 +3424,43 @@
       <c r="AX27">
         <v>0.83028189799088314</v>
       </c>
+      <c r="AZ27" s="13">
+        <v>8</v>
+      </c>
+      <c r="BA27">
+        <v>20000</v>
+      </c>
+      <c r="BB27">
+        <v>9</v>
+      </c>
+      <c r="BC27">
+        <v>0.94065254115938446</v>
+      </c>
+      <c r="BD27">
+        <v>3.4367920711214688</v>
+      </c>
+      <c r="BE27">
+        <v>1.9454979999999999</v>
+      </c>
+      <c r="BG27">
+        <v>3.5115795310554612</v>
+      </c>
     </row>
-    <row r="28" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="Q28" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="S28" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B29" s="6">
         <f>B28+1</f>
         <v>11</v>
@@ -3220,11 +3470,11 @@
         <v>11</v>
       </c>
       <c r="S29" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:50" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:59" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>12</v>
       </c>

</xml_diff>